<commit_message>
Added few things to risk list.
</commit_message>
<xml_diff>
--- a/LCOM Documents/Iteration2/LCOMRiskList.xlsx
+++ b/LCOM Documents/Iteration2/LCOMRiskList.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtuli\Dropbox\ITC303\2016\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deepakchand/Desktop/ITC303-9-Team1-Project/LCOM Documents/Iteration2/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBCF37B-B8F6-7E42-8016-3098726E28FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30090" windowHeight="15525" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -28,24 +29,37 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Risk_Tracking_Log!$1:$6</definedName>
     <definedName name="Risk_Area">DropDown_Elements!$A$2:$A$30</definedName>
   </definedNames>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>eze3</author>
     <author>e</author>
   </authors>
   <commentList>
-    <comment ref="A6" authorId="0" shapeId="0">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -54,7 +68,7 @@
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -62,21 +76,22 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>• Current Status:</t>
         </r>
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -85,9 +100,19 @@
         </r>
         <r>
           <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
             <b/>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -96,7 +121,7 @@
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -107,7 +132,7 @@
           <rPr>
             <b/>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -116,7 +141,7 @@
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -124,7 +149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0" shapeId="0">
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -207,21 +232,22 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="0" shapeId="0">
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>• Probability of Occurrence:</t>
         </r>
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -230,9 +256,19 @@
         </r>
         <r>
           <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
             <b/>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -241,7 +277,7 @@
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -252,7 +288,7 @@
           <rPr>
             <b/>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -261,7 +297,7 @@
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -272,7 +308,7 @@
           <rPr>
             <b/>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -281,7 +317,7 @@
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -289,13 +325,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="1" shapeId="0">
+    <comment ref="E6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -304,7 +340,7 @@
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -313,9 +349,19 @@
         </r>
         <r>
           <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
             <b/>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -324,7 +370,7 @@
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -335,7 +381,7 @@
           <rPr>
             <b/>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -344,7 +390,7 @@
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -355,7 +401,7 @@
           <rPr>
             <b/>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -364,7 +410,7 @@
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -372,7 +418,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="0" shapeId="0">
+    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -395,21 +441,22 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="1" shapeId="0">
+    <comment ref="G6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">• Project Impact:  </t>
         </r>
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -417,21 +464,22 @@
         </r>
       </text>
     </comment>
-    <comment ref="H6" authorId="0" shapeId="0">
+    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>• Risk Area:</t>
         </r>
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -439,7 +487,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I6" authorId="1" shapeId="0">
+    <comment ref="I6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
         <r>
           <rPr>
@@ -461,21 +509,22 @@
         </r>
       </text>
     </comment>
-    <comment ref="J6" authorId="1" shapeId="0">
+    <comment ref="J6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">• Triggers:  </t>
         </r>
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -483,21 +532,22 @@
         </r>
       </text>
     </comment>
-    <comment ref="K6" authorId="1" shapeId="0">
+    <comment ref="K6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Risk Response Strategy: </t>
         </r>
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -505,7 +555,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L6" authorId="0" shapeId="0">
+    <comment ref="L6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -528,7 +578,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M6" authorId="1" shapeId="0">
+    <comment ref="M6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -555,7 +605,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="114">
   <si>
     <t>ID</t>
   </si>
@@ -571,9 +621,6 @@
   <si>
     <t>Current
 Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> &lt;optional&gt;</t>
   </si>
   <si>
     <t>&lt;required&gt;</t>
@@ -1172,15 +1219,99 @@
   <si>
     <t>Complete the Project Name, NC, Project Manager Name, and Project Description fields</t>
   </si>
+  <si>
+    <t>ADHD Task Manager</t>
+  </si>
+  <si>
+    <t>Team 1</t>
+  </si>
+  <si>
+    <t>Task Manager app for individual with ADHD to complete tasks, gain rewards, and stay motivated.</t>
+  </si>
+  <si>
+    <t>A group member may leave course</t>
+  </si>
+  <si>
+    <t>Group members to shoulder extra tasks/responsibilities</t>
+  </si>
+  <si>
+    <t>Schedule                                           Project Resources</t>
+  </si>
+  <si>
+    <t>Tasks will need to be assgined to meet deadlines.                                                                Extra resources such as time will be required.</t>
+  </si>
+  <si>
+    <t>Team 1 gets notofied of a member leaving.</t>
+  </si>
+  <si>
+    <t>Transfer</t>
+  </si>
+  <si>
+    <t>Group meeting to distribute the task</t>
+  </si>
+  <si>
+    <t>Hinderence to starting Iteration 1.2.</t>
+  </si>
+  <si>
+    <t>Incomplete Iteration 1.1</t>
+  </si>
+  <si>
+    <t>Life-cycle Costs                                     Project Resources</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Iteration 1.2 start date approaches with incomplete Iteration 1.1</t>
+  </si>
+  <si>
+    <t>Tasks incomplete on date mentioned in the work plan</t>
+  </si>
+  <si>
+    <t>Team charter to be followed.</t>
+  </si>
+  <si>
+    <t>Secure user data if external database is used.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Life-cycle costs                                     Project Resources                                  Surety Considerations   </t>
+  </si>
+  <si>
+    <t>Teachical and knowledge competency not at the required level to implement security by deadline.</t>
+  </si>
+  <si>
+    <t>A week prior to dealine, this will be dropped/ not pursued.</t>
+  </si>
+  <si>
+    <t>Makign the app attractive aesthetically to keep user motivated</t>
+  </si>
+  <si>
+    <t>Requires skills beyond subject studied thus far: cybersecurity</t>
+  </si>
+  <si>
+    <t>If core use cases are not implemented, it would be hard to stay on track.</t>
+  </si>
+  <si>
+    <t>Feasibility                                                Project resources</t>
+  </si>
+  <si>
+    <t>Tangent  or non-core usecases impacts achievement of core use cases.</t>
+  </si>
+  <si>
+    <t>Core use cases are unaccounted for.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop non-core usecases. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1270,6 +1401,24 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1772,25 +1921,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1811,10 +1959,10 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1829,16 +1977,13 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1880,10 +2025,10 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1892,7 +2037,7 @@
     <xf numFmtId="49" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1901,28 +2046,25 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1940,7 +2082,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1957,7 +2099,7 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1969,27 +2111,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2008,9 +2141,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2019,19 +2149,16 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2050,6 +2177,13 @@
       <fill>
         <patternFill>
           <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="45"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2077,7 +2211,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor indexed="45"/>
+          <bgColor indexed="42"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2490,183 +2624,183 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="93" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="7.1640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="93" style="9" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="str">
+    <row r="1" spans="1:2" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="76" t="str">
         <f>Risk_Tracking_Log!A1</f>
         <v>RISK MANAGEMENT LOG</v>
       </c>
-      <c r="B1" s="84"/>
-    </row>
-    <row r="2" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="82" t="s">
+      <c r="B1" s="77"/>
+    </row>
+    <row r="2" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="75" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="12" x14ac:dyDescent="0.15">
+      <c r="A3" s="21"/>
+      <c r="B3" s="15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="12" x14ac:dyDescent="0.15">
+      <c r="A4" s="19"/>
+      <c r="B4" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="12" x14ac:dyDescent="0.15">
+      <c r="A5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B5" s="49" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="48" x14ac:dyDescent="0.15">
+      <c r="A6" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="72" x14ac:dyDescent="0.15">
+      <c r="A7" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="12" x14ac:dyDescent="0.15">
+      <c r="A8" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.15">
+      <c r="A9" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="49" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="12" x14ac:dyDescent="0.15">
+      <c r="A10" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="49" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="12" x14ac:dyDescent="0.15">
+      <c r="A11" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="12" x14ac:dyDescent="0.15">
+      <c r="A12" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="12" x14ac:dyDescent="0.15">
+      <c r="A13" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="49" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="12" x14ac:dyDescent="0.15">
+      <c r="A14" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="12" x14ac:dyDescent="0.15">
+      <c r="A15" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="12" x14ac:dyDescent="0.15">
+      <c r="A16" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="49" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="67" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="68" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="23"/>
-      <c r="B3" s="16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="20"/>
-      <c r="B4" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="52" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="52" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="67.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="52" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="53" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="52" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="52" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="21" t="s">
+    <row r="21" spans="1:2" ht="37" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="61" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="52" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="52" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="52" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="52" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="52" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="52" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="71" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="72" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21" s="24" t="s">
+      <c r="B25" s="22" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="57" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="24" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -2682,784 +2816,1146 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:O133"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="34" style="51" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" style="51" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="30.85546875" style="51" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="30.85546875" style="51" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="4"/>
-    <col min="15" max="15" width="6" style="4" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="3.1640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="34" style="48" customWidth="1"/>
+    <col min="8" max="8" width="22.1640625" style="48" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="30.83203125" style="48" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" style="48" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="30.83203125" style="48" customWidth="1"/>
+    <col min="15" max="15" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="7" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="6" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+        <v>24</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
       <c r="I1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-    </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="8" t="str">
+        <v>24</v>
+      </c>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+    </row>
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="32"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="7" t="str">
         <f>A2</f>
         <v>Project Name:</v>
       </c>
-      <c r="J2" s="32" t="str">
+      <c r="J2" s="30" t="str">
         <f>D2</f>
-        <v xml:space="preserve"> &lt;optional&gt;</v>
-      </c>
-      <c r="K2" s="38"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="70"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="70"/>
-    </row>
-    <row r="3" spans="1:21" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="38"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="9" t="str">
+        <v>ADHD Task Manager</v>
+      </c>
+      <c r="K2" s="36"/>
+    </row>
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="36"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="8" t="str">
         <f>A3</f>
         <v>National Center:</v>
       </c>
-      <c r="J3" s="36" t="str">
+      <c r="J3" s="34" t="str">
         <f>D3</f>
         <v>&lt;required&gt;</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
-      <c r="P3" s="70"/>
-      <c r="Q3" s="70"/>
-      <c r="R3" s="70"/>
-      <c r="S3" s="70"/>
-      <c r="T3" s="70"/>
-      <c r="U3" s="70"/>
-    </row>
-    <row r="4" spans="1:21" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="38"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="9" t="str">
+      <c r="K3" s="36"/>
+    </row>
+    <row r="4" spans="1:15" s="1" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="36"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="8" t="str">
         <f>A4</f>
         <v>Project Manager Name:</v>
       </c>
-      <c r="J4" s="39" t="str">
+      <c r="J4" s="37" t="str">
         <f>D4</f>
-        <v>&lt;required&gt;</v>
-      </c>
-      <c r="K4" s="38"/>
-      <c r="L4" s="70"/>
-      <c r="M4" s="70"/>
-      <c r="N4" s="70"/>
-      <c r="O4" s="70"/>
-      <c r="P4" s="70"/>
-      <c r="Q4" s="70"/>
-      <c r="R4" s="70"/>
-      <c r="S4" s="70"/>
-      <c r="T4" s="70"/>
-      <c r="U4" s="70"/>
-    </row>
-    <row r="5" spans="1:21" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="54" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="9" t="str">
+        <v>Team 1</v>
+      </c>
+      <c r="K4" s="36"/>
+    </row>
+    <row r="5" spans="1:15" s="1" customFormat="1" ht="61" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="29"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="8" t="str">
         <f>A5</f>
         <v>Project Description:</v>
       </c>
-      <c r="J5" s="81" t="str">
+      <c r="J5" s="51" t="str">
         <f>D5</f>
-        <v>&lt;required&gt;</v>
-      </c>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
-      <c r="M5" s="56"/>
-      <c r="N5" s="70"/>
-      <c r="O5" s="70"/>
-      <c r="P5" s="70"/>
-      <c r="Q5" s="70"/>
-      <c r="R5" s="70"/>
-      <c r="S5" s="70"/>
-      <c r="T5" s="70"/>
-      <c r="U5" s="70"/>
-    </row>
-    <row r="6" spans="1:21" s="3" customFormat="1" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="58" t="s">
+        <v>Task Manager app for individual with ADHD to complete tasks, gain rewards, and stay motivated.</v>
+      </c>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="53"/>
+    </row>
+    <row r="6" spans="1:15" s="3" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="57" t="s">
+      <c r="E6" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="59" t="s">
+      <c r="H6" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="59" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" s="62" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="57" t="s">
+      <c r="I6" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="J6" s="57" t="s">
+      <c r="K6" s="54" t="s">
+        <v>70</v>
+      </c>
+      <c r="L6" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="M6" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="K6" s="57" t="s">
-        <v>71</v>
-      </c>
-      <c r="L6" s="59" t="s">
-        <v>76</v>
-      </c>
-      <c r="M6" s="69" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="101.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
-      <c r="B7" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="27" t="s">
+    </row>
+    <row r="7" spans="1:15" ht="111" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="10"/>
+      <c r="B7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="68" t="str">
+      <c r="E7" s="65" t="str">
         <f>IF(OR(AND(B7&lt;&gt;"Closed",C7="High",D7="High"),AND(B7&lt;&gt;"Closed",C7="High",D7="Medium"),AND(B7&lt;&gt;"Closed",C7="Medium",D7="High")),"Red",IF(OR(AND(B7&lt;&gt;"Closed",C7="High",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Medium",D7="Medium"),AND(B7&lt;&gt;"Closed",C7="Low",D7="High")),"Yellow",IF(OR(AND(B7&lt;&gt;"Closed",C7="Medium",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Low",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Low",D7="Medium")),"Green",IF(B7="Closed","Closed",""))))</f>
         <v>Yellow</v>
       </c>
-      <c r="F7" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="G7" s="42" t="s">
+      <c r="F7" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="I7" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="H7" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="I7" s="42" t="s">
+      <c r="J7" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="J7" s="42" t="s">
+      <c r="K7" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="K7" s="80" t="s">
-        <v>70</v>
-      </c>
-      <c r="L7" s="42" t="s">
+      <c r="M7" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="M7" s="66" t="s">
-        <v>82</v>
-      </c>
-      <c r="O7" s="4" t="str">
+      <c r="O7" t="str">
         <f>IF(OR(AND(B7&lt;&gt;"Closed",C7="High",E7="High"), AND(B7&lt;&gt;"Closed",C7="High", E7="Medium"),AND(B7&lt;&gt;"Closed",C7="Medium",E7="High")),"Red",IF(OR(AND(B7&lt;&gt;"Closed",C7="High",E7="Low"), AND(B7&lt;&gt;"Closed",C7="Medium", E7="Medium"),AND(B7&lt;&gt;"Closed",C7="Low",E7="High")),"Yellow",IF(OR(AND(B7&lt;&gt;"Closed",C7="Medium",E7="Low"), AND(B7&lt;&gt;"Closed",C7="Low", E7="Low"),AND(B7&lt;&gt;"Closed",C7="Low",E7="Medium")),"Green","")))</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="27" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A8" s="10"/>
+      <c r="B8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="68" t="str">
+      <c r="E8" s="65" t="str">
         <f>IF(OR(AND(B8&lt;&gt;"Closed",C8="High",D8="High"),AND(B8&lt;&gt;"Closed",C8="High",D8="Medium"),AND(B8&lt;&gt;"Closed",C8="Medium",D8="High")),"Red",IF(OR(AND(B8&lt;&gt;"Closed",C8="High",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Medium",D8="Medium"),AND(B8&lt;&gt;"Closed",C8="Low",D8="High")),"Yellow",IF(OR(AND(B8&lt;&gt;"Closed",C8="Medium",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Low",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Low",D8="Medium")),"Green",IF(B8="Closed","Closed",""))))</f>
         <v>Yellow</v>
       </c>
-      <c r="F8" s="42"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="75"/>
-      <c r="J8" s="67"/>
-      <c r="K8" s="80"/>
-      <c r="L8" s="75"/>
-      <c r="M8" s="43"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
-      <c r="B9" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="27" t="s">
+      <c r="F8" s="40"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="69"/>
+      <c r="M8" s="41"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A9" s="10"/>
+      <c r="B9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="68" t="str">
+      <c r="E9" s="65" t="str">
         <f>IF(OR(AND(B9&lt;&gt;"Closed",C9="High",D9="High"),AND(B9&lt;&gt;"Closed",C9="High",D9="Medium"),AND(B9&lt;&gt;"Closed",C9="Medium",D9="High")),"Red",IF(OR(AND(B9&lt;&gt;"Closed",C9="High",D9="Low"),AND(B9&lt;&gt;"Closed",C9="Medium",D9="Medium"),AND(B9&lt;&gt;"Closed",C9="Low",D9="High")),"Yellow",IF(OR(AND(B9&lt;&gt;"Closed",C9="Medium",D9="Low"),AND(B9&lt;&gt;"Closed",C9="Low",D9="Low"),AND(B9&lt;&gt;"Closed",C9="Low",D9="Medium")),"Green",IF(B9="Closed","Closed",""))))</f>
         <v>Green</v>
       </c>
-      <c r="F9" s="42"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="80"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="43"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="68" t="str">
+      <c r="F9" s="40"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="64"/>
+      <c r="K9" s="74"/>
+      <c r="L9" s="69"/>
+      <c r="M9" s="41"/>
+    </row>
+    <row r="10" spans="1:15" ht="53" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="10"/>
+      <c r="B10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="65" t="str">
         <f t="shared" ref="E10:E35" si="0">IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="High"),AND(B10&lt;&gt;"Closed",C10="High",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="High")),"Red",IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Low",D10="High")),"Yellow",IF(OR(AND(B10&lt;&gt;"Closed",C10="Medium",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Medium")),"Green",IF(B10="Closed","Closed",""))))</f>
-        <v/>
-      </c>
-      <c r="F10" s="42"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="75"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="80"/>
-      <c r="L10" s="77"/>
-      <c r="M10" s="44"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="68" t="str">
+        <v>Yellow</v>
+      </c>
+      <c r="F10" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="G10" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="H10" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="I10" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="K10" s="74" t="s">
+        <v>94</v>
+      </c>
+      <c r="L10" s="71" t="s">
+        <v>1</v>
+      </c>
+      <c r="M10" s="45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="24" x14ac:dyDescent="0.15">
+      <c r="A11" s="10"/>
+      <c r="B11" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="65" t="str">
+        <f t="shared" si="0"/>
+        <v>Closed</v>
+      </c>
+      <c r="F11" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="G11" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="H11" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="I11" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="J11" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="K11" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="L11" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" s="44" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="36" x14ac:dyDescent="0.15">
+      <c r="A12" s="11"/>
+      <c r="B12" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="65" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
+      </c>
+      <c r="F12" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="G12" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="H12" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="I12" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="J12" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="K12" s="74"/>
+      <c r="L12" s="71"/>
+      <c r="M12" s="45"/>
+      <c r="N12" s="78"/>
+    </row>
+    <row r="13" spans="1:15" ht="24" x14ac:dyDescent="0.15">
+      <c r="A13" s="11"/>
+      <c r="B13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="65" t="str">
+        <f t="shared" si="0"/>
+        <v>Green</v>
+      </c>
+      <c r="F13" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="G13" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="H13" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="I13" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="J13" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="K13" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="L13" s="71"/>
+      <c r="M13" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="N13" s="78"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A14" s="11"/>
+      <c r="B14" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F11" s="45"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="80"/>
-      <c r="L11" s="78"/>
-      <c r="M11" s="47"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="68" t="str">
+      <c r="F14" s="43"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="74"/>
+      <c r="L14" s="71"/>
+      <c r="M14" s="45"/>
+      <c r="N14" s="78"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A15" s="11"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F12" s="46"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="67"/>
-      <c r="K12" s="80"/>
-      <c r="L12" s="77"/>
-      <c r="M12" s="48"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="68" t="str">
+      <c r="F15" s="43"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="74"/>
+      <c r="L15" s="71"/>
+      <c r="M15" s="45"/>
+      <c r="N15" s="78"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A16" s="11"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F13" s="46"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="75"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="80"/>
-      <c r="L13" s="77"/>
-      <c r="M13" s="48"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="68" t="str">
+      <c r="F16" s="43"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="74"/>
+      <c r="L16" s="71"/>
+      <c r="M16" s="45"/>
+      <c r="N16" s="78"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A17" s="11"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F14" s="46"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="75"/>
-      <c r="J14" s="67"/>
-      <c r="K14" s="80"/>
-      <c r="L14" s="77"/>
-      <c r="M14" s="48"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="68" t="str">
+      <c r="F17" s="43"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="74"/>
+      <c r="L17" s="71"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="78"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A18" s="11"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F15" s="46"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="75"/>
-      <c r="J15" s="67"/>
-      <c r="K15" s="80"/>
-      <c r="L15" s="77"/>
-      <c r="M15" s="48"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="68" t="str">
+      <c r="F18" s="43"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="74"/>
+      <c r="L18" s="71"/>
+      <c r="M18" s="45"/>
+      <c r="N18" s="78"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A19" s="11"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F16" s="46"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="80"/>
-      <c r="L16" s="77"/>
-      <c r="M16" s="48"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="12"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="68" t="str">
+      <c r="F19" s="43"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="74"/>
+      <c r="L19" s="71"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="78"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A20" s="11"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F17" s="46"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="75"/>
-      <c r="J17" s="67"/>
-      <c r="K17" s="80"/>
-      <c r="L17" s="77"/>
-      <c r="M17" s="48"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="68" t="str">
+      <c r="F20" s="43"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="74"/>
+      <c r="L20" s="71"/>
+      <c r="M20" s="45"/>
+      <c r="N20" s="78"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A21" s="11"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F18" s="46"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="75"/>
-      <c r="J18" s="67"/>
-      <c r="K18" s="80"/>
-      <c r="L18" s="77"/>
-      <c r="M18" s="48"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="12"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="68" t="str">
+      <c r="F21" s="43"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="74"/>
+      <c r="L21" s="71"/>
+      <c r="M21" s="45"/>
+      <c r="N21" s="78"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A22" s="11"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F19" s="46"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="67"/>
-      <c r="K19" s="80"/>
-      <c r="L19" s="77"/>
-      <c r="M19" s="48"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="68" t="str">
+      <c r="F22" s="43"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="74"/>
+      <c r="L22" s="71"/>
+      <c r="M22" s="45"/>
+      <c r="N22" s="78"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A23" s="11"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F20" s="46"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="75"/>
-      <c r="J20" s="67"/>
-      <c r="K20" s="80"/>
-      <c r="L20" s="77"/>
-      <c r="M20" s="48"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="12"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="68" t="str">
+      <c r="F23" s="43"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="74"/>
+      <c r="L23" s="71"/>
+      <c r="M23" s="45"/>
+      <c r="N23" s="78"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A24" s="11"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F21" s="46"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="75"/>
-      <c r="J21" s="67"/>
-      <c r="K21" s="80"/>
-      <c r="L21" s="77"/>
-      <c r="M21" s="48"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="12"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="68" t="str">
+      <c r="F24" s="43"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="74"/>
+      <c r="L24" s="71"/>
+      <c r="M24" s="45"/>
+      <c r="N24" s="78"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A25" s="11"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F22" s="46"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="75"/>
-      <c r="J22" s="67"/>
-      <c r="K22" s="80"/>
-      <c r="L22" s="77"/>
-      <c r="M22" s="48"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="12"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="68" t="str">
+      <c r="F25" s="43"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="74"/>
+      <c r="L25" s="71"/>
+      <c r="M25" s="45"/>
+      <c r="N25" s="78"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A26" s="11"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F23" s="46"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="75"/>
-      <c r="J23" s="67"/>
-      <c r="K23" s="80"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="48"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="12"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="68" t="str">
+      <c r="F26" s="43"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="74"/>
+      <c r="L26" s="71"/>
+      <c r="M26" s="45"/>
+      <c r="N26" s="78"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A27" s="11"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F24" s="46"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="75"/>
-      <c r="J24" s="67"/>
-      <c r="K24" s="80"/>
-      <c r="L24" s="77"/>
-      <c r="M24" s="48"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="12"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="68" t="str">
+      <c r="F27" s="43"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="74"/>
+      <c r="L27" s="71"/>
+      <c r="M27" s="45"/>
+      <c r="N27" s="78"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A28" s="11"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F25" s="46"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="75"/>
-      <c r="J25" s="67"/>
-      <c r="K25" s="80"/>
-      <c r="L25" s="77"/>
-      <c r="M25" s="48"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="12"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="68" t="str">
+      <c r="F28" s="43"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="74"/>
+      <c r="L28" s="71"/>
+      <c r="M28" s="45"/>
+      <c r="N28" s="78"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A29" s="11"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F26" s="46"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="75"/>
-      <c r="J26" s="67"/>
-      <c r="K26" s="80"/>
-      <c r="L26" s="77"/>
-      <c r="M26" s="48"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="12"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="68" t="str">
+      <c r="F29" s="43"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="74"/>
+      <c r="L29" s="71"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="78"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A30" s="11"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F27" s="46"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="75"/>
-      <c r="J27" s="67"/>
-      <c r="K27" s="80"/>
-      <c r="L27" s="77"/>
-      <c r="M27" s="48"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="12"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="68" t="str">
+      <c r="F30" s="43"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="74"/>
+      <c r="L30" s="71"/>
+      <c r="M30" s="45"/>
+      <c r="N30" s="78"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A31" s="11"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F28" s="46"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="75"/>
-      <c r="J28" s="67"/>
-      <c r="K28" s="80"/>
-      <c r="L28" s="77"/>
-      <c r="M28" s="48"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="12"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="68" t="str">
+      <c r="F31" s="43"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="74"/>
+      <c r="L31" s="71"/>
+      <c r="M31" s="45"/>
+      <c r="N31" s="78"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A32" s="11"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F29" s="46"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="75"/>
-      <c r="J29" s="67"/>
-      <c r="K29" s="80"/>
-      <c r="L29" s="77"/>
-      <c r="M29" s="48"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="12"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="68" t="str">
+      <c r="F32" s="43"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="74"/>
+      <c r="L32" s="71"/>
+      <c r="M32" s="45"/>
+      <c r="N32" s="78"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A33" s="11"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F30" s="46"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="75"/>
-      <c r="J30" s="67"/>
-      <c r="K30" s="80"/>
-      <c r="L30" s="77"/>
-      <c r="M30" s="48"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="12"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="68" t="str">
+      <c r="F33" s="43"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="42"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="74"/>
+      <c r="L33" s="71"/>
+      <c r="M33" s="45"/>
+      <c r="N33" s="78"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A34" s="11"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F31" s="46"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="75"/>
-      <c r="J31" s="67"/>
-      <c r="K31" s="80"/>
-      <c r="L31" s="77"/>
-      <c r="M31" s="48"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="12"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="68" t="str">
+      <c r="F34" s="43"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="42"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="74"/>
+      <c r="L34" s="71"/>
+      <c r="M34" s="45"/>
+      <c r="N34" s="78"/>
+    </row>
+    <row r="35" spans="1:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="12"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F32" s="46"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="75"/>
-      <c r="J32" s="67"/>
-      <c r="K32" s="80"/>
-      <c r="L32" s="77"/>
-      <c r="M32" s="48"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="12"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="68" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F33" s="46"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="75"/>
-      <c r="J33" s="67"/>
-      <c r="K33" s="80"/>
-      <c r="L33" s="77"/>
-      <c r="M33" s="48"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="12"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="68" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F34" s="46"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="41"/>
-      <c r="I34" s="75"/>
-      <c r="J34" s="67"/>
-      <c r="K34" s="80"/>
-      <c r="L34" s="77"/>
-      <c r="M34" s="48"/>
-    </row>
-    <row r="35" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="63"/>
-      <c r="D35" s="63"/>
-      <c r="E35" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F35" s="49"/>
-      <c r="G35" s="64"/>
-      <c r="H35" s="64"/>
-      <c r="I35" s="73"/>
-      <c r="J35" s="74"/>
-      <c r="K35" s="76"/>
-      <c r="L35" s="79"/>
-      <c r="M35" s="50"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="61"/>
+      <c r="H35" s="61"/>
+      <c r="I35" s="46"/>
+      <c r="J35" s="79"/>
+      <c r="K35" s="70"/>
+      <c r="L35" s="73"/>
+      <c r="M35" s="47"/>
+      <c r="N35" s="78"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="N36" s="78"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="N37" s="78"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="N38" s="78"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="N39" s="78"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="N40" s="78"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="N41" s="78"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="N42" s="78"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="N43" s="78"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="N44" s="78"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="N45" s="78"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="N46" s="78"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="N47" s="78"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="N48" s="78"/>
+    </row>
+    <row r="49" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N49" s="78"/>
+    </row>
+    <row r="50" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N50" s="78"/>
+    </row>
+    <row r="51" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N51" s="78"/>
+    </row>
+    <row r="52" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N52" s="78"/>
+    </row>
+    <row r="53" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N53" s="78"/>
+    </row>
+    <row r="54" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N54" s="78"/>
+    </row>
+    <row r="55" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N55" s="78"/>
+    </row>
+    <row r="56" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N56" s="78"/>
+    </row>
+    <row r="57" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N57" s="78"/>
+    </row>
+    <row r="58" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N58" s="78"/>
+    </row>
+    <row r="59" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N59" s="78"/>
+    </row>
+    <row r="60" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N60" s="78"/>
+    </row>
+    <row r="61" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N61" s="78"/>
+    </row>
+    <row r="62" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N62" s="78"/>
+    </row>
+    <row r="63" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N63" s="78"/>
+    </row>
+    <row r="64" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N64" s="78"/>
+    </row>
+    <row r="65" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N65" s="78"/>
+    </row>
+    <row r="66" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N66" s="78"/>
+    </row>
+    <row r="67" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N67" s="78"/>
+    </row>
+    <row r="68" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N68" s="78"/>
+    </row>
+    <row r="69" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N69" s="78"/>
+    </row>
+    <row r="70" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N70" s="78"/>
+    </row>
+    <row r="71" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N71" s="78"/>
+    </row>
+    <row r="72" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N72" s="78"/>
+    </row>
+    <row r="73" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N73" s="78"/>
+    </row>
+    <row r="74" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N74" s="78"/>
+    </row>
+    <row r="75" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N75" s="78"/>
+    </row>
+    <row r="76" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N76" s="78"/>
+    </row>
+    <row r="77" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N77" s="78"/>
+    </row>
+    <row r="78" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N78" s="78"/>
+    </row>
+    <row r="79" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N79" s="78"/>
+    </row>
+    <row r="80" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N80" s="78"/>
+    </row>
+    <row r="81" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N81" s="78"/>
+    </row>
+    <row r="82" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N82" s="78"/>
+    </row>
+    <row r="83" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N83" s="78"/>
+    </row>
+    <row r="84" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N84" s="78"/>
+    </row>
+    <row r="85" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N85" s="78"/>
+    </row>
+    <row r="86" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N86" s="78"/>
+    </row>
+    <row r="87" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N87" s="78"/>
+    </row>
+    <row r="88" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N88" s="78"/>
+    </row>
+    <row r="89" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N89" s="78"/>
+    </row>
+    <row r="90" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N90" s="78"/>
+    </row>
+    <row r="91" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N91" s="78"/>
+    </row>
+    <row r="92" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N92" s="78"/>
+    </row>
+    <row r="93" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N93" s="78"/>
+    </row>
+    <row r="94" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N94" s="78"/>
+    </row>
+    <row r="95" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N95" s="78"/>
+    </row>
+    <row r="96" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N96" s="78"/>
+    </row>
+    <row r="97" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N97" s="78"/>
+    </row>
+    <row r="98" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N98" s="78"/>
+    </row>
+    <row r="99" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N99" s="78"/>
+    </row>
+    <row r="100" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N100" s="78"/>
+    </row>
+    <row r="101" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N101" s="78"/>
+    </row>
+    <row r="102" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N102" s="78"/>
+    </row>
+    <row r="103" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N103" s="78"/>
+    </row>
+    <row r="104" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N104" s="78"/>
+    </row>
+    <row r="105" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N105" s="78"/>
+    </row>
+    <row r="106" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N106" s="78"/>
+    </row>
+    <row r="107" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N107" s="78"/>
+    </row>
+    <row r="108" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N108" s="78"/>
+    </row>
+    <row r="109" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N109" s="78"/>
+    </row>
+    <row r="110" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N110" s="78"/>
+    </row>
+    <row r="111" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N111" s="78"/>
+    </row>
+    <row r="112" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N112" s="78"/>
+    </row>
+    <row r="113" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N113" s="78"/>
+    </row>
+    <row r="114" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N114" s="78"/>
+    </row>
+    <row r="115" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N115" s="78"/>
+    </row>
+    <row r="116" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N116" s="78"/>
+    </row>
+    <row r="117" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N117" s="78"/>
+    </row>
+    <row r="118" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N118" s="78"/>
+    </row>
+    <row r="119" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N119" s="78"/>
+    </row>
+    <row r="120" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N120" s="78"/>
+    </row>
+    <row r="121" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N121" s="78"/>
+    </row>
+    <row r="122" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N122" s="78"/>
+    </row>
+    <row r="123" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N123" s="78"/>
+    </row>
+    <row r="124" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N124" s="78"/>
+    </row>
+    <row r="125" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N125" s="78"/>
+    </row>
+    <row r="126" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N126" s="78"/>
+    </row>
+    <row r="127" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N127" s="78"/>
+    </row>
+    <row r="128" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N128" s="78"/>
+    </row>
+    <row r="129" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N129" s="78"/>
+    </row>
+    <row r="130" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N130" s="78"/>
+    </row>
+    <row r="131" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N131" s="78"/>
+    </row>
+    <row r="132" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N132" s="78"/>
+    </row>
+    <row r="133" spans="14:14" x14ac:dyDescent="0.15">
+      <c r="N133" s="78"/>
     </row>
   </sheetData>
-  <autoFilter ref="B6:D6"/>
+  <autoFilter ref="B6:D6" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="C36:E65536 C1:E1 B6:C6 B7:B35">
+  <conditionalFormatting sqref="B7:B35 B6:C6 C1:E1 C36:E65536">
     <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
@@ -3470,47 +3966,47 @@
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L10:L35">
-    <cfRule type="cellIs" dxfId="7" priority="4" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="C7:D35">
+    <cfRule type="cellIs" dxfId="7" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="9" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" stopIfTrue="1" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7:E35">
+    <cfRule type="cellIs" dxfId="4" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Yellow"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Red"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"Green"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L10:L35">
+    <cfRule type="cellIs" dxfId="1" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7:E35">
-    <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Red"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Yellow"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="8" stopIfTrue="1" operator="equal">
-      <formula>"Green"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C7:D35">
-    <cfRule type="cellIs" dxfId="2" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L10:L35 C7:D35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L10:L35 C7:D35" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H35" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>Risk_Area</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B35" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K35" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"Acceptance,Avoidance,Contingency,Mitigation,Transfer"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3524,116 +4020,116 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+    <row r="1" spans="1:1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="57" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" s="58" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="61" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3" s="58" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="61" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" s="58" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="61" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5" s="58" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="61" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A6" s="58" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="61" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A7" s="58" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="61" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A8" s="58" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="61" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A9" s="58" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="61" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A10" s="58" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="61" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A11" s="58" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="61" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A12" s="58" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="61" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A13" s="58" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="61" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A14" s="58" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="61" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A15" s="58" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="61" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A16" s="58" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="61" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A17" s="58" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="61" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A18" s="58" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="61" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A19" s="58" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="61" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A20" s="58" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="61" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add few more items to LCOMRiskList.xlsx.
</commit_message>
<xml_diff>
--- a/LCOM Documents/Iteration2/LCOMRiskList.xlsx
+++ b/LCOM Documents/Iteration2/LCOMRiskList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deepakchand/Desktop/ITC303-9-Team1-Project/LCOM Documents/Iteration2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBCF37B-B8F6-7E42-8016-3098726E28FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720E46BE-8E21-CA41-AB08-09F008766D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Risk_Tracking_Log!$B$6:$D$6</definedName>
     <definedName name="as">[1]DropDown_Elements!$A$2:$A$30</definedName>
     <definedName name="OLE_LINK1" localSheetId="1">Risk_Tracking_Log!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Risk_Tracking_Log!$A$1:$M$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Risk_Tracking_Log!$A$1:$M$33</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Risk_Tracking_Log!$1:$6</definedName>
     <definedName name="Risk_Area">DropDown_Elements!$A$2:$A$30</definedName>
   </definedNames>
@@ -605,7 +605,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="145">
   <si>
     <t>ID</t>
   </si>
@@ -621,9 +621,6 @@
   <si>
     <t>Current
 Status</t>
-  </si>
-  <si>
-    <t>&lt;required&gt;</t>
   </si>
   <si>
     <t>Project Name:</t>
@@ -1302,6 +1299,102 @@
   </si>
   <si>
     <t xml:space="preserve">Drop non-core usecases. </t>
+  </si>
+  <si>
+    <t>Compatibility issues with different IDEs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Significant impact because some members might have to redo certain components therefore taking longer than expected. </t>
+  </si>
+  <si>
+    <t>Members using diffeent IDEs but no issues yet, while working on the same main remote branch.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If a week before Iteration 2.1, there are issues with working on individual branches, refer to contigency plan. </t>
+  </si>
+  <si>
+    <t>Contingency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High level of customisation such as font colour. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Such features may add additional difficulties. </t>
+  </si>
+  <si>
+    <t>Find resources to address this. As a last resort, everyone uses one IDE.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reliability of Systems                          Schedule                                                             Overall project failure                            Technology                         </t>
+  </si>
+  <si>
+    <t>Schedule approaches deadline, and core cases are not implemented.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 weeks prior to deadlin, if core use cases are not implemented, then drop non-core usecases. </t>
+  </si>
+  <si>
+    <t>Acceptance</t>
+  </si>
+  <si>
+    <t>Accept  core use-cases only.</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Communication Sqlite database in Android Studio</t>
+  </si>
+  <si>
+    <t>Kotlin is a new language being used. It is vital for the app to comminucate with Sqlite database to add/retirieve data</t>
+  </si>
+  <si>
+    <t>Data/Information                                   Overall project failure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data will need to be added/retrieved from Sqlite dataabse; If core uses cases requires this but the know how is missing. </t>
+  </si>
+  <si>
+    <t>A week before deadlin, there is no evidence of logical communication with local database.</t>
+  </si>
+  <si>
+    <t>Team members to look for resources and implement the logical connection between the app and the Sqlite database</t>
+  </si>
+  <si>
+    <t>Communication breakdown in group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Without comminucation, there is little to no awareness how things are progressing. </t>
+  </si>
+  <si>
+    <t>Schedule                                                Overall project failure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lack of communication especially items that are central to the app's core usecases. </t>
+  </si>
+  <si>
+    <t>Meetings to be conducted on scheduled times.</t>
+  </si>
+  <si>
+    <t>Team charter to be followed and actioned.</t>
+  </si>
+  <si>
+    <t>Legal issues regarding user data protection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project may fail if adequate security is not implemented. Lack of cyber security knowledge.  </t>
+  </si>
+  <si>
+    <t>Schedule                                                 Project resources                                   Overall project failure</t>
+  </si>
+  <si>
+    <t>Cyber security skill set not identified as the deadline approaches.</t>
+  </si>
+  <si>
+    <t>2 weeks prior to deadline, if not skills/resources identified, refer to contigency plan.</t>
+  </si>
+  <si>
+    <t>Do not pursue storing data in external database.</t>
   </si>
 </sst>
 </file>
@@ -1921,7 +2014,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2041,9 +2134,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2108,9 +2198,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2122,9 +2209,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2183,13 +2267,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor indexed="45"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor indexed="43"/>
         </patternFill>
       </fill>
@@ -2204,6 +2281,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor indexed="47"/>
         </patternFill>
       </fill>
@@ -2211,7 +2295,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor indexed="42"/>
+          <bgColor indexed="45"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2639,168 +2723,168 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="76" t="str">
+      <c r="A1" s="73" t="str">
         <f>Risk_Tracking_Log!A1</f>
         <v>RISK MANAGEMENT LOG</v>
       </c>
-      <c r="B1" s="77"/>
+      <c r="B1" s="74"/>
     </row>
     <row r="2" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="75" t="s">
-        <v>13</v>
+      <c r="A2" s="72" t="s">
+        <v>12</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12" x14ac:dyDescent="0.15">
       <c r="A3" s="21"/>
       <c r="B3" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12" x14ac:dyDescent="0.15">
       <c r="A4" s="19"/>
       <c r="B4" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12" x14ac:dyDescent="0.15">
       <c r="A5" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="49" t="s">
-        <v>83</v>
+        <v>13</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="48" x14ac:dyDescent="0.15">
       <c r="A6" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="49" t="s">
-        <v>68</v>
+        <v>14</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="72" x14ac:dyDescent="0.15">
       <c r="A7" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="49" t="s">
-        <v>53</v>
+        <v>15</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="12" x14ac:dyDescent="0.15">
       <c r="A8" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="50" t="s">
-        <v>49</v>
+        <v>16</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.15">
       <c r="A9" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="49" t="s">
-        <v>73</v>
+        <v>17</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="12" x14ac:dyDescent="0.15">
       <c r="A10" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="49" t="s">
-        <v>46</v>
+        <v>18</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="12" x14ac:dyDescent="0.15">
       <c r="A11" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="49" t="s">
-        <v>58</v>
+        <v>19</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="12" x14ac:dyDescent="0.15">
       <c r="A12" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="49" t="s">
-        <v>48</v>
+        <v>61</v>
+      </c>
+      <c r="B12" s="48" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="12" x14ac:dyDescent="0.15">
       <c r="A13" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="49" t="s">
-        <v>59</v>
+        <v>62</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12" x14ac:dyDescent="0.15">
       <c r="A14" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14" s="49" t="s">
-        <v>60</v>
+        <v>63</v>
+      </c>
+      <c r="B14" s="48" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="12" x14ac:dyDescent="0.15">
       <c r="A15" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="B15" s="49" t="s">
-        <v>72</v>
+        <v>64</v>
+      </c>
+      <c r="B15" s="48" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="12" x14ac:dyDescent="0.15">
       <c r="A16" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="B16" s="49" t="s">
-        <v>74</v>
+        <v>65</v>
+      </c>
+      <c r="B16" s="48" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="67" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="68" t="s">
-        <v>61</v>
+      <c r="A17" s="65" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="66" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="37" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="61" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A25" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2817,10 +2901,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O133"/>
+  <dimension ref="A1:O131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2830,17 +2915,17 @@
     <col min="3" max="3" width="10.5" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="34" style="48" customWidth="1"/>
-    <col min="8" max="8" width="22.1640625" style="48" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="30.83203125" style="48" customWidth="1"/>
-    <col min="11" max="11" width="12.83203125" style="48" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="30.83203125" style="48" customWidth="1"/>
+    <col min="6" max="7" width="34" style="47" customWidth="1"/>
+    <col min="8" max="8" width="22.1640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="30.83203125" style="47" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" style="47" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="30.83203125" style="47" customWidth="1"/>
     <col min="15" max="15" width="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="6" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -2850,7 +2935,7 @@
       <c r="G1" s="27"/>
       <c r="H1" s="27"/>
       <c r="I1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J1" s="28"/>
       <c r="K1" s="28"/>
@@ -2859,12 +2944,12 @@
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
       <c r="D2" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E2" s="32"/>
       <c r="F2" s="31"/>
@@ -2882,12 +2967,12 @@
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="33"/>
       <c r="D3" s="34" t="s">
-        <v>5</v>
+        <v>126</v>
       </c>
       <c r="E3" s="36"/>
       <c r="F3" s="35"/>
@@ -2899,18 +2984,18 @@
       </c>
       <c r="J3" s="34" t="str">
         <f>D3</f>
-        <v>&lt;required&gt;</v>
+        <v>Australia</v>
       </c>
       <c r="K3" s="36"/>
     </row>
     <row r="4" spans="1:15" s="1" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="33"/>
       <c r="D4" s="37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E4" s="36"/>
       <c r="F4" s="35"/>
@@ -2928,74 +3013,74 @@
     </row>
     <row r="5" spans="1:15" s="1" customFormat="1" ht="61" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="38"/>
-      <c r="D5" s="51" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
+      <c r="D5" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
       <c r="I5" s="8" t="str">
         <f>A5</f>
         <v>Project Description:</v>
       </c>
-      <c r="J5" s="51" t="str">
+      <c r="J5" s="50" t="str">
         <f>D5</f>
         <v>Task Manager app for individual with ADHD to complete tasks, gain rewards, and stay motivated.</v>
       </c>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="53"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="52"/>
     </row>
     <row r="6" spans="1:15" s="3" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="E6" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="54" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="56" t="s">
+      <c r="H6" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="56" t="s">
-        <v>57</v>
-      </c>
-      <c r="H6" s="59" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="54" t="s">
+      <c r="I6" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="J6" s="54" t="s">
+      <c r="K6" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="L6" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="M6" s="64" t="s">
         <v>51</v>
-      </c>
-      <c r="K6" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="L6" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="M6" s="66" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="111" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10"/>
       <c r="B7" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>1</v>
@@ -3003,959 +3088,1019 @@
       <c r="D7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="65" t="str">
+      <c r="E7" s="63" t="str">
         <f>IF(OR(AND(B7&lt;&gt;"Closed",C7="High",D7="High"),AND(B7&lt;&gt;"Closed",C7="High",D7="Medium"),AND(B7&lt;&gt;"Closed",C7="Medium",D7="High")),"Red",IF(OR(AND(B7&lt;&gt;"Closed",C7="High",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Medium",D7="Medium"),AND(B7&lt;&gt;"Closed",C7="Low",D7="High")),"Yellow",IF(OR(AND(B7&lt;&gt;"Closed",C7="Medium",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Low",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Low",D7="Medium")),"Green",IF(B7="Closed","Closed",""))))</f>
         <v>Yellow</v>
       </c>
       <c r="F7" s="40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G7" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="H7" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="I7" s="40" t="s">
+      <c r="J7" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="J7" s="40" t="s">
+      <c r="K7" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="L7" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="K7" s="74" t="s">
-        <v>69</v>
-      </c>
-      <c r="L7" s="40" t="s">
+      <c r="M7" s="62" t="s">
         <v>80</v>
-      </c>
-      <c r="M7" s="63" t="s">
-        <v>81</v>
       </c>
       <c r="O7" t="str">
         <f>IF(OR(AND(B7&lt;&gt;"Closed",C7="High",E7="High"), AND(B7&lt;&gt;"Closed",C7="High", E7="Medium"),AND(B7&lt;&gt;"Closed",C7="Medium",E7="High")),"Red",IF(OR(AND(B7&lt;&gt;"Closed",C7="High",E7="Low"), AND(B7&lt;&gt;"Closed",C7="Medium", E7="Medium"),AND(B7&lt;&gt;"Closed",C7="Low",E7="High")),"Yellow",IF(OR(AND(B7&lt;&gt;"Closed",C7="Medium",E7="Low"), AND(B7&lt;&gt;"Closed",C7="Low", E7="Low"),AND(B7&lt;&gt;"Closed",C7="Low",E7="Medium")),"Green","")))</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" ht="53" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10"/>
       <c r="B8" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="65" t="str">
-        <f>IF(OR(AND(B8&lt;&gt;"Closed",C8="High",D8="High"),AND(B8&lt;&gt;"Closed",C8="High",D8="Medium"),AND(B8&lt;&gt;"Closed",C8="Medium",D8="High")),"Red",IF(OR(AND(B8&lt;&gt;"Closed",C8="High",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Medium",D8="Medium"),AND(B8&lt;&gt;"Closed",C8="Low",D8="High")),"Yellow",IF(OR(AND(B8&lt;&gt;"Closed",C8="Medium",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Low",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Low",D8="Medium")),"Green",IF(B8="Closed","Closed",""))))</f>
+        <v>3</v>
+      </c>
+      <c r="E8" s="63" t="str">
+        <f t="shared" ref="E8:E33" si="0">IF(OR(AND(B8&lt;&gt;"Closed",C8="High",D8="High"),AND(B8&lt;&gt;"Closed",C8="High",D8="Medium"),AND(B8&lt;&gt;"Closed",C8="Medium",D8="High")),"Red",IF(OR(AND(B8&lt;&gt;"Closed",C8="High",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Medium",D8="Medium"),AND(B8&lt;&gt;"Closed",C8="Low",D8="High")),"Yellow",IF(OR(AND(B8&lt;&gt;"Closed",C8="Medium",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Low",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Low",D8="Medium")),"Green",IF(B8="Closed","Closed",""))))</f>
         <v>Yellow</v>
       </c>
-      <c r="F8" s="40"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="74"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="41"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="F8" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="I8" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="J8" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="K8" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="L8" s="68" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="44" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
       <c r="B9" s="13" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="65" t="str">
-        <f>IF(OR(AND(B9&lt;&gt;"Closed",C9="High",D9="High"),AND(B9&lt;&gt;"Closed",C9="High",D9="Medium"),AND(B9&lt;&gt;"Closed",C9="Medium",D9="High")),"Red",IF(OR(AND(B9&lt;&gt;"Closed",C9="High",D9="Low"),AND(B9&lt;&gt;"Closed",C9="Medium",D9="Medium"),AND(B9&lt;&gt;"Closed",C9="Low",D9="High")),"Yellow",IF(OR(AND(B9&lt;&gt;"Closed",C9="Medium",D9="Low"),AND(B9&lt;&gt;"Closed",C9="Low",D9="Low"),AND(B9&lt;&gt;"Closed",C9="Low",D9="Medium")),"Green",IF(B9="Closed","Closed",""))))</f>
-        <v>Green</v>
-      </c>
-      <c r="F9" s="40"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="64"/>
-      <c r="K9" s="74"/>
-      <c r="L9" s="69"/>
-      <c r="M9" s="41"/>
-    </row>
-    <row r="10" spans="1:15" ht="53" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="D9" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="63" t="str">
+        <f t="shared" si="0"/>
+        <v>Closed</v>
+      </c>
+      <c r="F9" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="G9" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="I9" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="J9" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="K9" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="L9" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="43" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="36" x14ac:dyDescent="0.15">
+      <c r="A10" s="11"/>
       <c r="B10" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="63" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="G10" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="H10" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="I10" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="J10" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="K10" s="71"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="75"/>
+    </row>
+    <row r="11" spans="1:15" ht="24" x14ac:dyDescent="0.15">
+      <c r="A11" s="11"/>
+      <c r="B11" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="65" t="str">
-        <f t="shared" ref="E10:E35" si="0">IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="High"),AND(B10&lt;&gt;"Closed",C10="High",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="High")),"Red",IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Low",D10="High")),"Yellow",IF(OR(AND(B10&lt;&gt;"Closed",C10="Medium",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Medium")),"Green",IF(B10="Closed","Closed",""))))</f>
-        <v>Yellow</v>
-      </c>
-      <c r="F10" s="43" t="s">
-        <v>89</v>
-      </c>
-      <c r="G10" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="H10" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="I10" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="J10" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="K10" s="74" t="s">
-        <v>94</v>
-      </c>
-      <c r="L10" s="71" t="s">
-        <v>1</v>
-      </c>
-      <c r="M10" s="45" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="A11" s="10"/>
-      <c r="B11" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="65" t="str">
+      <c r="D11" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="63" t="str">
         <f t="shared" si="0"/>
-        <v>Closed</v>
+        <v>Green</v>
       </c>
       <c r="F11" s="42" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="G11" s="39" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="H11" s="39" t="s">
-        <v>98</v>
-      </c>
-      <c r="I11" s="42" t="s">
-        <v>100</v>
+        <v>109</v>
+      </c>
+      <c r="I11" s="41" t="s">
+        <v>110</v>
       </c>
       <c r="J11" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="K11" s="74" t="s">
-        <v>69</v>
-      </c>
-      <c r="L11" s="72" t="s">
-        <v>1</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="K11" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="L11" s="68"/>
       <c r="M11" s="44" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="36" x14ac:dyDescent="0.15">
+        <v>112</v>
+      </c>
+      <c r="N11" s="75"/>
+    </row>
+    <row r="12" spans="1:15" ht="48" x14ac:dyDescent="0.15">
       <c r="A12" s="11"/>
       <c r="B12" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="65" t="str">
+        <v>1</v>
+      </c>
+      <c r="E12" s="63" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
-      <c r="F12" s="43" t="s">
-        <v>103</v>
+      <c r="F12" s="42" t="s">
+        <v>113</v>
       </c>
       <c r="G12" s="39" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="H12" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="I12" s="42" t="s">
-        <v>105</v>
+        <v>121</v>
+      </c>
+      <c r="I12" s="41" t="s">
+        <v>115</v>
       </c>
       <c r="J12" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="K12" s="74"/>
-      <c r="L12" s="71"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="78"/>
+        <v>116</v>
+      </c>
+      <c r="K12" s="71" t="s">
+        <v>117</v>
+      </c>
+      <c r="L12" s="68" t="s">
+        <v>1</v>
+      </c>
+      <c r="M12" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="N12" s="75"/>
     </row>
     <row r="13" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A13" s="11"/>
       <c r="B13" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="63" t="str">
+        <f t="shared" si="0"/>
+        <v>Yellow</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="G13" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="H13" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="J13" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="K13" s="71" t="s">
+        <v>124</v>
+      </c>
+      <c r="L13" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="65" t="str">
-        <f t="shared" si="0"/>
-        <v>Green</v>
-      </c>
-      <c r="F13" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="G13" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="H13" s="39" t="s">
-        <v>110</v>
-      </c>
-      <c r="I13" s="42" t="s">
-        <v>111</v>
-      </c>
-      <c r="J13" s="39" t="s">
-        <v>112</v>
-      </c>
-      <c r="K13" s="74" t="s">
-        <v>69</v>
-      </c>
-      <c r="L13" s="71"/>
-      <c r="M13" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="N13" s="78"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="M13" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="N13" s="75"/>
+    </row>
+    <row r="14" spans="1:15" ht="36" x14ac:dyDescent="0.15">
       <c r="A14" s="11"/>
       <c r="B14" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="65" t="str">
+        <v>8</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="63" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F14" s="43"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="74"/>
-      <c r="L14" s="71"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="78"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+        <v>Yellow</v>
+      </c>
+      <c r="F14" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="G14" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="H14" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="I14" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="J14" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="K14" s="71" t="s">
+        <v>117</v>
+      </c>
+      <c r="L14" s="68" t="s">
+        <v>1</v>
+      </c>
+      <c r="M14" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="N14" s="75"/>
+    </row>
+    <row r="15" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A15" s="11"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="65" t="str">
+      <c r="B15" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="63" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F15" s="43"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="74"/>
-      <c r="L15" s="71"/>
-      <c r="M15" s="45"/>
-      <c r="N15" s="78"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+        <v>Red</v>
+      </c>
+      <c r="F15" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="G15" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="H15" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="I15" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="J15" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="K15" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="L15" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="M15" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="N15" s="75"/>
+    </row>
+    <row r="16" spans="1:15" ht="36" x14ac:dyDescent="0.15">
       <c r="A16" s="11"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="65" t="str">
+      <c r="B16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="63" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F16" s="43"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="74"/>
-      <c r="L16" s="71"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="78"/>
+        <v>Yellow</v>
+      </c>
+      <c r="F16" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="G16" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="H16" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="I16" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="J16" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="K16" s="71" t="s">
+        <v>117</v>
+      </c>
+      <c r="L16" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="N16" s="75"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A17" s="11"/>
       <c r="B17" s="13"/>
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="65" t="str">
+      <c r="E17" s="63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F17" s="43"/>
+      <c r="F17" s="42"/>
       <c r="G17" s="39"/>
       <c r="H17" s="39"/>
-      <c r="I17" s="42"/>
+      <c r="I17" s="41"/>
       <c r="J17" s="39"/>
-      <c r="K17" s="74"/>
-      <c r="L17" s="71"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="78"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="68"/>
+      <c r="M17" s="44"/>
+      <c r="N17" s="75"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A18" s="11"/>
       <c r="B18" s="13"/>
       <c r="C18" s="25"/>
       <c r="D18" s="25"/>
-      <c r="E18" s="65" t="str">
+      <c r="E18" s="63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F18" s="43"/>
+      <c r="F18" s="42"/>
       <c r="G18" s="39"/>
       <c r="H18" s="39"/>
-      <c r="I18" s="42"/>
+      <c r="I18" s="41"/>
       <c r="J18" s="39"/>
-      <c r="K18" s="74"/>
-      <c r="L18" s="71"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="78"/>
+      <c r="K18" s="71"/>
+      <c r="L18" s="68"/>
+      <c r="M18" s="44"/>
+      <c r="N18" s="75"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A19" s="11"/>
       <c r="B19" s="13"/>
       <c r="C19" s="25"/>
       <c r="D19" s="25"/>
-      <c r="E19" s="65" t="str">
+      <c r="E19" s="63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F19" s="43"/>
+      <c r="F19" s="42"/>
       <c r="G19" s="39"/>
       <c r="H19" s="39"/>
-      <c r="I19" s="42"/>
+      <c r="I19" s="41"/>
       <c r="J19" s="39"/>
-      <c r="K19" s="74"/>
-      <c r="L19" s="71"/>
-      <c r="M19" s="45"/>
-      <c r="N19" s="78"/>
+      <c r="K19" s="71"/>
+      <c r="L19" s="68"/>
+      <c r="M19" s="44"/>
+      <c r="N19" s="75"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A20" s="11"/>
       <c r="B20" s="13"/>
       <c r="C20" s="25"/>
       <c r="D20" s="25"/>
-      <c r="E20" s="65" t="str">
+      <c r="E20" s="63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F20" s="43"/>
+      <c r="F20" s="42"/>
       <c r="G20" s="39"/>
       <c r="H20" s="39"/>
-      <c r="I20" s="42"/>
+      <c r="I20" s="41"/>
       <c r="J20" s="39"/>
-      <c r="K20" s="74"/>
-      <c r="L20" s="71"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="78"/>
+      <c r="K20" s="71"/>
+      <c r="L20" s="68"/>
+      <c r="M20" s="44"/>
+      <c r="N20" s="75"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A21" s="11"/>
       <c r="B21" s="13"/>
       <c r="C21" s="25"/>
       <c r="D21" s="25"/>
-      <c r="E21" s="65" t="str">
+      <c r="E21" s="63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F21" s="43"/>
+      <c r="F21" s="42"/>
       <c r="G21" s="39"/>
       <c r="H21" s="39"/>
-      <c r="I21" s="42"/>
+      <c r="I21" s="41"/>
       <c r="J21" s="39"/>
-      <c r="K21" s="74"/>
-      <c r="L21" s="71"/>
-      <c r="M21" s="45"/>
-      <c r="N21" s="78"/>
+      <c r="K21" s="71"/>
+      <c r="L21" s="68"/>
+      <c r="M21" s="44"/>
+      <c r="N21" s="75"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A22" s="11"/>
       <c r="B22" s="13"/>
       <c r="C22" s="25"/>
       <c r="D22" s="25"/>
-      <c r="E22" s="65" t="str">
+      <c r="E22" s="63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F22" s="43"/>
+      <c r="F22" s="42"/>
       <c r="G22" s="39"/>
       <c r="H22" s="39"/>
-      <c r="I22" s="42"/>
+      <c r="I22" s="41"/>
       <c r="J22" s="39"/>
-      <c r="K22" s="74"/>
-      <c r="L22" s="71"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="78"/>
+      <c r="K22" s="71"/>
+      <c r="L22" s="68"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="75"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A23" s="11"/>
       <c r="B23" s="13"/>
       <c r="C23" s="25"/>
       <c r="D23" s="25"/>
-      <c r="E23" s="65" t="str">
+      <c r="E23" s="63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F23" s="43"/>
+      <c r="F23" s="42"/>
       <c r="G23" s="39"/>
       <c r="H23" s="39"/>
-      <c r="I23" s="42"/>
+      <c r="I23" s="41"/>
       <c r="J23" s="39"/>
-      <c r="K23" s="74"/>
-      <c r="L23" s="71"/>
-      <c r="M23" s="45"/>
-      <c r="N23" s="78"/>
+      <c r="K23" s="71"/>
+      <c r="L23" s="68"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="75"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A24" s="11"/>
       <c r="B24" s="13"/>
       <c r="C24" s="25"/>
       <c r="D24" s="25"/>
-      <c r="E24" s="65" t="str">
+      <c r="E24" s="63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F24" s="43"/>
+      <c r="F24" s="42"/>
       <c r="G24" s="39"/>
       <c r="H24" s="39"/>
-      <c r="I24" s="42"/>
+      <c r="I24" s="41"/>
       <c r="J24" s="39"/>
-      <c r="K24" s="74"/>
-      <c r="L24" s="71"/>
-      <c r="M24" s="45"/>
-      <c r="N24" s="78"/>
+      <c r="K24" s="71"/>
+      <c r="L24" s="68"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="75"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A25" s="11"/>
       <c r="B25" s="13"/>
       <c r="C25" s="25"/>
       <c r="D25" s="25"/>
-      <c r="E25" s="65" t="str">
+      <c r="E25" s="63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F25" s="43"/>
+      <c r="F25" s="42"/>
       <c r="G25" s="39"/>
       <c r="H25" s="39"/>
-      <c r="I25" s="42"/>
+      <c r="I25" s="41"/>
       <c r="J25" s="39"/>
-      <c r="K25" s="74"/>
-      <c r="L25" s="71"/>
-      <c r="M25" s="45"/>
-      <c r="N25" s="78"/>
+      <c r="K25" s="71"/>
+      <c r="L25" s="68"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="75"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A26" s="11"/>
       <c r="B26" s="13"/>
       <c r="C26" s="25"/>
       <c r="D26" s="25"/>
-      <c r="E26" s="65" t="str">
+      <c r="E26" s="63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F26" s="43"/>
+      <c r="F26" s="42"/>
       <c r="G26" s="39"/>
       <c r="H26" s="39"/>
-      <c r="I26" s="42"/>
+      <c r="I26" s="41"/>
       <c r="J26" s="39"/>
-      <c r="K26" s="74"/>
-      <c r="L26" s="71"/>
-      <c r="M26" s="45"/>
-      <c r="N26" s="78"/>
+      <c r="K26" s="71"/>
+      <c r="L26" s="68"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="75"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A27" s="11"/>
       <c r="B27" s="13"/>
       <c r="C27" s="25"/>
       <c r="D27" s="25"/>
-      <c r="E27" s="65" t="str">
+      <c r="E27" s="63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F27" s="43"/>
+      <c r="F27" s="42"/>
       <c r="G27" s="39"/>
       <c r="H27" s="39"/>
-      <c r="I27" s="42"/>
+      <c r="I27" s="41"/>
       <c r="J27" s="39"/>
-      <c r="K27" s="74"/>
-      <c r="L27" s="71"/>
-      <c r="M27" s="45"/>
-      <c r="N27" s="78"/>
+      <c r="K27" s="71"/>
+      <c r="L27" s="68"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="75"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A28" s="11"/>
       <c r="B28" s="13"/>
       <c r="C28" s="25"/>
       <c r="D28" s="25"/>
-      <c r="E28" s="65" t="str">
+      <c r="E28" s="63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F28" s="43"/>
+      <c r="F28" s="42"/>
       <c r="G28" s="39"/>
       <c r="H28" s="39"/>
-      <c r="I28" s="42"/>
+      <c r="I28" s="41"/>
       <c r="J28" s="39"/>
-      <c r="K28" s="74"/>
-      <c r="L28" s="71"/>
-      <c r="M28" s="45"/>
-      <c r="N28" s="78"/>
+      <c r="K28" s="71"/>
+      <c r="L28" s="68"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="75"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A29" s="11"/>
       <c r="B29" s="13"/>
       <c r="C29" s="25"/>
       <c r="D29" s="25"/>
-      <c r="E29" s="65" t="str">
+      <c r="E29" s="63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F29" s="43"/>
+      <c r="F29" s="42"/>
       <c r="G29" s="39"/>
       <c r="H29" s="39"/>
-      <c r="I29" s="42"/>
+      <c r="I29" s="41"/>
       <c r="J29" s="39"/>
-      <c r="K29" s="74"/>
-      <c r="L29" s="71"/>
-      <c r="M29" s="45"/>
-      <c r="N29" s="78"/>
+      <c r="K29" s="71"/>
+      <c r="L29" s="68"/>
+      <c r="M29" s="44"/>
+      <c r="N29" s="75"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A30" s="11"/>
       <c r="B30" s="13"/>
       <c r="C30" s="25"/>
       <c r="D30" s="25"/>
-      <c r="E30" s="65" t="str">
+      <c r="E30" s="63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F30" s="43"/>
+      <c r="F30" s="42"/>
       <c r="G30" s="39"/>
       <c r="H30" s="39"/>
-      <c r="I30" s="42"/>
+      <c r="I30" s="41"/>
       <c r="J30" s="39"/>
-      <c r="K30" s="74"/>
-      <c r="L30" s="71"/>
-      <c r="M30" s="45"/>
-      <c r="N30" s="78"/>
+      <c r="K30" s="71"/>
+      <c r="L30" s="68"/>
+      <c r="M30" s="44"/>
+      <c r="N30" s="75"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A31" s="11"/>
       <c r="B31" s="13"/>
       <c r="C31" s="25"/>
       <c r="D31" s="25"/>
-      <c r="E31" s="65" t="str">
+      <c r="E31" s="63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F31" s="43"/>
+      <c r="F31" s="42"/>
       <c r="G31" s="39"/>
       <c r="H31" s="39"/>
-      <c r="I31" s="42"/>
+      <c r="I31" s="41"/>
       <c r="J31" s="39"/>
-      <c r="K31" s="74"/>
-      <c r="L31" s="71"/>
-      <c r="M31" s="45"/>
-      <c r="N31" s="78"/>
+      <c r="K31" s="71"/>
+      <c r="L31" s="68"/>
+      <c r="M31" s="44"/>
+      <c r="N31" s="75"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A32" s="11"/>
       <c r="B32" s="13"/>
       <c r="C32" s="25"/>
       <c r="D32" s="25"/>
-      <c r="E32" s="65" t="str">
+      <c r="E32" s="63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F32" s="43"/>
+      <c r="F32" s="42"/>
       <c r="G32" s="39"/>
       <c r="H32" s="39"/>
-      <c r="I32" s="42"/>
+      <c r="I32" s="41"/>
       <c r="J32" s="39"/>
-      <c r="K32" s="74"/>
-      <c r="L32" s="71"/>
-      <c r="M32" s="45"/>
-      <c r="N32" s="78"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A33" s="11"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="65" t="str">
+      <c r="K32" s="71"/>
+      <c r="L32" s="68"/>
+      <c r="M32" s="44"/>
+      <c r="N32" s="75"/>
+    </row>
+    <row r="33" spans="1:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="12"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F33" s="43"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="42"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="74"/>
-      <c r="L33" s="71"/>
-      <c r="M33" s="45"/>
-      <c r="N33" s="78"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="76"/>
+      <c r="K33" s="67"/>
+      <c r="L33" s="70"/>
+      <c r="M33" s="46"/>
+      <c r="N33" s="75"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A34" s="11"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="65" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F34" s="43"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="42"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="74"/>
-      <c r="L34" s="71"/>
-      <c r="M34" s="45"/>
-      <c r="N34" s="78"/>
-    </row>
-    <row r="35" spans="1:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="12"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F35" s="46"/>
-      <c r="G35" s="61"/>
-      <c r="H35" s="61"/>
-      <c r="I35" s="46"/>
-      <c r="J35" s="79"/>
-      <c r="K35" s="70"/>
-      <c r="L35" s="73"/>
-      <c r="M35" s="47"/>
-      <c r="N35" s="78"/>
+      <c r="N34" s="75"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="N35" s="75"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N36" s="78"/>
+      <c r="N36" s="75"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N37" s="78"/>
+      <c r="N37" s="75"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N38" s="78"/>
+      <c r="N38" s="75"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N39" s="78"/>
+      <c r="N39" s="75"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N40" s="78"/>
+      <c r="N40" s="75"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N41" s="78"/>
+      <c r="N41" s="75"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N42" s="78"/>
+      <c r="N42" s="75"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N43" s="78"/>
+      <c r="N43" s="75"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N44" s="78"/>
+      <c r="N44" s="75"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N45" s="78"/>
+      <c r="N45" s="75"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N46" s="78"/>
+      <c r="N46" s="75"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N47" s="78"/>
+      <c r="N47" s="75"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N48" s="78"/>
+      <c r="N48" s="75"/>
     </row>
     <row r="49" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N49" s="78"/>
+      <c r="N49" s="75"/>
     </row>
     <row r="50" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N50" s="78"/>
+      <c r="N50" s="75"/>
     </row>
     <row r="51" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N51" s="78"/>
+      <c r="N51" s="75"/>
     </row>
     <row r="52" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N52" s="78"/>
+      <c r="N52" s="75"/>
     </row>
     <row r="53" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N53" s="78"/>
+      <c r="N53" s="75"/>
     </row>
     <row r="54" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N54" s="78"/>
+      <c r="N54" s="75"/>
     </row>
     <row r="55" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N55" s="78"/>
+      <c r="N55" s="75"/>
     </row>
     <row r="56" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N56" s="78"/>
+      <c r="N56" s="75"/>
     </row>
     <row r="57" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N57" s="78"/>
+      <c r="N57" s="75"/>
     </row>
     <row r="58" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N58" s="78"/>
+      <c r="N58" s="75"/>
     </row>
     <row r="59" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N59" s="78"/>
+      <c r="N59" s="75"/>
     </row>
     <row r="60" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N60" s="78"/>
+      <c r="N60" s="75"/>
     </row>
     <row r="61" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N61" s="78"/>
+      <c r="N61" s="75"/>
     </row>
     <row r="62" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N62" s="78"/>
+      <c r="N62" s="75"/>
     </row>
     <row r="63" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N63" s="78"/>
+      <c r="N63" s="75"/>
     </row>
     <row r="64" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N64" s="78"/>
+      <c r="N64" s="75"/>
     </row>
     <row r="65" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N65" s="78"/>
+      <c r="N65" s="75"/>
     </row>
     <row r="66" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N66" s="78"/>
+      <c r="N66" s="75"/>
     </row>
     <row r="67" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N67" s="78"/>
+      <c r="N67" s="75"/>
     </row>
     <row r="68" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N68" s="78"/>
+      <c r="N68" s="75"/>
     </row>
     <row r="69" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N69" s="78"/>
+      <c r="N69" s="75"/>
     </row>
     <row r="70" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N70" s="78"/>
+      <c r="N70" s="75"/>
     </row>
     <row r="71" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N71" s="78"/>
+      <c r="N71" s="75"/>
     </row>
     <row r="72" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N72" s="78"/>
+      <c r="N72" s="75"/>
     </row>
     <row r="73" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N73" s="78"/>
+      <c r="N73" s="75"/>
     </row>
     <row r="74" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N74" s="78"/>
+      <c r="N74" s="75"/>
     </row>
     <row r="75" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N75" s="78"/>
+      <c r="N75" s="75"/>
     </row>
     <row r="76" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N76" s="78"/>
+      <c r="N76" s="75"/>
     </row>
     <row r="77" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N77" s="78"/>
+      <c r="N77" s="75"/>
     </row>
     <row r="78" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N78" s="78"/>
+      <c r="N78" s="75"/>
     </row>
     <row r="79" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N79" s="78"/>
+      <c r="N79" s="75"/>
     </row>
     <row r="80" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N80" s="78"/>
+      <c r="N80" s="75"/>
     </row>
     <row r="81" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N81" s="78"/>
+      <c r="N81" s="75"/>
     </row>
     <row r="82" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N82" s="78"/>
+      <c r="N82" s="75"/>
     </row>
     <row r="83" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N83" s="78"/>
+      <c r="N83" s="75"/>
     </row>
     <row r="84" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N84" s="78"/>
+      <c r="N84" s="75"/>
     </row>
     <row r="85" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N85" s="78"/>
+      <c r="N85" s="75"/>
     </row>
     <row r="86" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N86" s="78"/>
+      <c r="N86" s="75"/>
     </row>
     <row r="87" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N87" s="78"/>
+      <c r="N87" s="75"/>
     </row>
     <row r="88" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N88" s="78"/>
+      <c r="N88" s="75"/>
     </row>
     <row r="89" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N89" s="78"/>
+      <c r="N89" s="75"/>
     </row>
     <row r="90" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N90" s="78"/>
+      <c r="N90" s="75"/>
     </row>
     <row r="91" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N91" s="78"/>
+      <c r="N91" s="75"/>
     </row>
     <row r="92" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N92" s="78"/>
+      <c r="N92" s="75"/>
     </row>
     <row r="93" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N93" s="78"/>
+      <c r="N93" s="75"/>
     </row>
     <row r="94" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N94" s="78"/>
+      <c r="N94" s="75"/>
     </row>
     <row r="95" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N95" s="78"/>
+      <c r="N95" s="75"/>
     </row>
     <row r="96" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N96" s="78"/>
+      <c r="N96" s="75"/>
     </row>
     <row r="97" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N97" s="78"/>
+      <c r="N97" s="75"/>
     </row>
     <row r="98" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N98" s="78"/>
+      <c r="N98" s="75"/>
     </row>
     <row r="99" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N99" s="78"/>
+      <c r="N99" s="75"/>
     </row>
     <row r="100" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N100" s="78"/>
+      <c r="N100" s="75"/>
     </row>
     <row r="101" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N101" s="78"/>
+      <c r="N101" s="75"/>
     </row>
     <row r="102" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N102" s="78"/>
+      <c r="N102" s="75"/>
     </row>
     <row r="103" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N103" s="78"/>
+      <c r="N103" s="75"/>
     </row>
     <row r="104" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N104" s="78"/>
+      <c r="N104" s="75"/>
     </row>
     <row r="105" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N105" s="78"/>
+      <c r="N105" s="75"/>
     </row>
     <row r="106" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N106" s="78"/>
+      <c r="N106" s="75"/>
     </row>
     <row r="107" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N107" s="78"/>
+      <c r="N107" s="75"/>
     </row>
     <row r="108" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N108" s="78"/>
+      <c r="N108" s="75"/>
     </row>
     <row r="109" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N109" s="78"/>
+      <c r="N109" s="75"/>
     </row>
     <row r="110" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N110" s="78"/>
+      <c r="N110" s="75"/>
     </row>
     <row r="111" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N111" s="78"/>
+      <c r="N111" s="75"/>
     </row>
     <row r="112" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N112" s="78"/>
+      <c r="N112" s="75"/>
     </row>
     <row r="113" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N113" s="78"/>
+      <c r="N113" s="75"/>
     </row>
     <row r="114" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N114" s="78"/>
+      <c r="N114" s="75"/>
     </row>
     <row r="115" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N115" s="78"/>
+      <c r="N115" s="75"/>
     </row>
     <row r="116" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N116" s="78"/>
+      <c r="N116" s="75"/>
     </row>
     <row r="117" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N117" s="78"/>
+      <c r="N117" s="75"/>
     </row>
     <row r="118" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N118" s="78"/>
+      <c r="N118" s="75"/>
     </row>
     <row r="119" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N119" s="78"/>
+      <c r="N119" s="75"/>
     </row>
     <row r="120" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N120" s="78"/>
+      <c r="N120" s="75"/>
     </row>
     <row r="121" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N121" s="78"/>
+      <c r="N121" s="75"/>
     </row>
     <row r="122" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N122" s="78"/>
+      <c r="N122" s="75"/>
     </row>
     <row r="123" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N123" s="78"/>
+      <c r="N123" s="75"/>
     </row>
     <row r="124" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N124" s="78"/>
+      <c r="N124" s="75"/>
     </row>
     <row r="125" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N125" s="78"/>
+      <c r="N125" s="75"/>
     </row>
     <row r="126" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N126" s="78"/>
+      <c r="N126" s="75"/>
     </row>
     <row r="127" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N127" s="78"/>
+      <c r="N127" s="75"/>
     </row>
     <row r="128" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N128" s="78"/>
+      <c r="N128" s="75"/>
     </row>
     <row r="129" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N129" s="78"/>
+      <c r="N129" s="75"/>
     </row>
     <row r="130" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N130" s="78"/>
+      <c r="N130" s="75"/>
     </row>
     <row r="131" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N131" s="78"/>
-    </row>
-    <row r="132" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N132" s="78"/>
-    </row>
-    <row r="133" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N133" s="78"/>
+      <c r="N131" s="75"/>
     </row>
   </sheetData>
   <autoFilter ref="B6:D6" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="B7:B35 B6:C6 C1:E1 C36:E65536">
+  <conditionalFormatting sqref="B6:C6 C1:E1 C34:E65534 B7:B33">
     <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
@@ -3966,29 +4111,29 @@
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:D35">
-    <cfRule type="cellIs" dxfId="7" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Low"</formula>
+  <conditionalFormatting sqref="C7:D33">
+    <cfRule type="cellIs" dxfId="7" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"High"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"High"</formula>
+    <cfRule type="cellIs" dxfId="5" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7:E35">
-    <cfRule type="cellIs" dxfId="4" priority="7" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="E7:E33">
+    <cfRule type="cellIs" dxfId="4" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Red"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Yellow"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Red"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L10:L35">
+  <conditionalFormatting sqref="L8:L33">
     <cfRule type="cellIs" dxfId="1" priority="4" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
@@ -3997,16 +4142,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L10:L35 C7:D35" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L8:L33 C7:D33" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H35" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H33" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>Risk_Area</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B35" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B33" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K35" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K33" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"Acceptance,Avoidance,Contingency,Mitigation,Transfer"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4033,103 +4178,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="56" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" s="57" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A2" s="58" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3" s="57" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A3" s="58" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" s="57" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A4" s="58" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5" s="57" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A5" s="58" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A6" s="57" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A6" s="58" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A7" s="57" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A7" s="58" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A8" s="57" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A8" s="58" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A9" s="57" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A9" s="58" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A10" s="57" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A10" s="58" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A11" s="57" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A11" s="58" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A12" s="57" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A12" s="58" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A13" s="57" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A13" s="58" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A14" s="57" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A14" s="58" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A15" s="57" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A15" s="58" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A16" s="57" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A16" s="58" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A17" s="57" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A17" s="58" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A18" s="57" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A18" s="58" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A19" s="57" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A19" s="58" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A20" s="57" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A20" s="58" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added risk items to  LCOMRiskList.xlsx. Item 1.1 and 1.2
</commit_message>
<xml_diff>
--- a/LCOM Documents/Iteration2/LCOMRiskList.xlsx
+++ b/LCOM Documents/Iteration2/LCOMRiskList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deepakchand/Desktop/ITC303-9-Team1-Project/LCOM Documents/Iteration2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B85394-925E-EA42-BB4C-6C00760DD72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4F6160-4210-7D4D-90D2-B0AE565D133A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -493,15 +493,16 @@
           <rPr>
             <b/>
             <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>• Symptoms:</t>
         </r>
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -586,6 +587,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">• Contingency Plan:  </t>
         </r>
@@ -605,7 +607,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="159">
   <si>
     <t>ID</t>
   </si>
@@ -1223,9 +1225,6 @@
     <t>Team 1</t>
   </si>
   <si>
-    <t>Task Manager app for individual with ADHD to complete tasks, gain rewards, and stay motivated.</t>
-  </si>
-  <si>
     <t>A group member may leave course</t>
   </si>
   <si>
@@ -1413,6 +1412,33 @@
   </si>
   <si>
     <t>Team members identify minimum agreed core use cases.</t>
+  </si>
+  <si>
+    <t>Task Manager app for individuals with ADHD to complete tasks, gain rewards, and stay motivated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Functional accuracy </t>
+  </si>
+  <si>
+    <t>Apps accuracy is paramount for users.</t>
+  </si>
+  <si>
+    <t>Surety Considerations                         data/information                                    ds</t>
+  </si>
+  <si>
+    <t>Tests show inaccurate outcomes.</t>
+  </si>
+  <si>
+    <t>2 weeks prior to deadline, if  inaccuracy is not addressed refer to contigency plan.</t>
+  </si>
+  <si>
+    <t>Team members to work collaborately to address functional inaccuracies.</t>
+  </si>
+  <si>
+    <t>Avoidance</t>
+  </si>
+  <si>
+    <t>Just use local storage on device.</t>
   </si>
 </sst>
 </file>
@@ -1422,7 +1448,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1443,6 +1469,7 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="7"/>
@@ -1472,12 +1499,6 @@
       <color indexed="9"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
     </font>
     <font>
       <b/>
@@ -2032,7 +2053,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2109,13 +2130,13 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2175,10 +2196,10 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2199,7 +2220,7 @@
     <xf numFmtId="49" fontId="6" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2225,7 +2246,7 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2246,14 +2267,29 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2285,6 +2321,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor indexed="45"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor indexed="43"/>
         </patternFill>
       </fill>
@@ -2299,13 +2342,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor indexed="47"/>
         </patternFill>
       </fill>
@@ -2313,7 +2349,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor indexed="45"/>
+          <bgColor indexed="42"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2741,11 +2777,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="str">
+      <c r="A1" s="75" t="str">
         <f>Risk_Tracking_Log!A1</f>
         <v>RISK MANAGEMENT LOG</v>
       </c>
-      <c r="B1" s="74"/>
+      <c r="B1" s="76"/>
     </row>
     <row r="2" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="72" t="s">
@@ -2921,9 +2957,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2990,7 +3026,7 @@
       <c r="B3" s="33"/>
       <c r="C3" s="33"/>
       <c r="D3" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E3" s="36"/>
       <c r="F3" s="35"/>
@@ -3035,8 +3071,8 @@
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="38"/>
-      <c r="D5" s="50" t="s">
-        <v>87</v>
+      <c r="D5" s="77" t="s">
+        <v>150</v>
       </c>
       <c r="E5" s="51"/>
       <c r="F5" s="51"/>
@@ -3048,7 +3084,7 @@
       </c>
       <c r="J5" s="50" t="str">
         <f>D5</f>
-        <v>Task Manager app for individual with ADHD to complete tasks, gain rewards, and stay motivated.</v>
+        <v>Task Manager app for individuals with ADHD to complete tasks, gain rewards, and stay motivated.</v>
       </c>
       <c r="K5" s="51"/>
       <c r="L5" s="51"/>
@@ -3155,34 +3191,34 @@
         <v>Yellow</v>
       </c>
       <c r="F8" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="G8" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="H8" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="I8" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="I8" s="41" t="s">
+      <c r="J8" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="J8" s="39" t="s">
+      <c r="K8" s="71" t="s">
         <v>92</v>
-      </c>
-      <c r="K8" s="71" t="s">
-        <v>93</v>
       </c>
       <c r="L8" s="68" t="s">
         <v>1</v>
       </c>
       <c r="M8" s="44" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
       <c r="B9" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>1</v>
@@ -3195,19 +3231,19 @@
         <v>Closed</v>
       </c>
       <c r="F9" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="G9" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="H9" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="G9" s="39" t="s">
-        <v>95</v>
-      </c>
-      <c r="H9" s="39" t="s">
-        <v>97</v>
-      </c>
       <c r="I9" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="J9" s="39" t="s">
         <v>99</v>
-      </c>
-      <c r="J9" s="39" t="s">
-        <v>100</v>
       </c>
       <c r="K9" s="71" t="s">
         <v>68</v>
@@ -3216,7 +3252,7 @@
         <v>1</v>
       </c>
       <c r="M9" s="43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="36" x14ac:dyDescent="0.15">
@@ -3235,24 +3271,30 @@
         <v>Red</v>
       </c>
       <c r="F10" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="G10" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="H10" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="G10" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="H10" s="39" t="s">
+      <c r="I10" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="I10" s="41" t="s">
+      <c r="J10" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="J10" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="K10" s="71"/>
-      <c r="L10" s="68"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="75"/>
+      <c r="K10" s="71" t="s">
+        <v>157</v>
+      </c>
+      <c r="L10" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="M10" s="81" t="s">
+        <v>158</v>
+      </c>
+      <c r="N10" s="73"/>
     </row>
     <row r="11" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A11" s="11"/>
@@ -3270,28 +3312,30 @@
         <v>Green</v>
       </c>
       <c r="F11" s="42" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G11" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="H11" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="H11" s="39" t="s">
+      <c r="I11" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="I11" s="41" t="s">
+      <c r="J11" s="39" t="s">
         <v>110</v>
-      </c>
-      <c r="J11" s="39" t="s">
-        <v>111</v>
       </c>
       <c r="K11" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="L11" s="68"/>
+      <c r="L11" s="68" t="s">
+        <v>3</v>
+      </c>
       <c r="M11" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="N11" s="75"/>
+        <v>111</v>
+      </c>
+      <c r="N11" s="73"/>
     </row>
     <row r="12" spans="1:15" ht="48" x14ac:dyDescent="0.15">
       <c r="A12" s="11"/>
@@ -3309,30 +3353,30 @@
         <v>Red</v>
       </c>
       <c r="F12" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="G12" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="G12" s="39" t="s">
+      <c r="H12" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="I12" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="H12" s="39" t="s">
-        <v>121</v>
-      </c>
-      <c r="I12" s="41" t="s">
+      <c r="J12" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="J12" s="39" t="s">
+      <c r="K12" s="71" t="s">
         <v>116</v>
-      </c>
-      <c r="K12" s="71" t="s">
-        <v>117</v>
       </c>
       <c r="L12" s="68" t="s">
         <v>1</v>
       </c>
       <c r="M12" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="N12" s="75"/>
+        <v>119</v>
+      </c>
+      <c r="N12" s="73"/>
     </row>
     <row r="13" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A13" s="11"/>
@@ -3350,30 +3394,30 @@
         <v>Yellow</v>
       </c>
       <c r="F13" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" s="39" t="s">
         <v>118</v>
-      </c>
-      <c r="G13" s="39" t="s">
-        <v>119</v>
       </c>
       <c r="H13" s="39" t="s">
         <v>26</v>
       </c>
       <c r="I13" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="J13" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="J13" s="39" t="s">
+      <c r="K13" s="71" t="s">
         <v>123</v>
-      </c>
-      <c r="K13" s="71" t="s">
-        <v>124</v>
       </c>
       <c r="L13" s="68" t="s">
         <v>2</v>
       </c>
       <c r="M13" s="44" t="s">
-        <v>125</v>
-      </c>
-      <c r="N13" s="75"/>
+        <v>124</v>
+      </c>
+      <c r="N13" s="73"/>
     </row>
     <row r="14" spans="1:15" ht="36" x14ac:dyDescent="0.15">
       <c r="A14" s="11"/>
@@ -3391,30 +3435,30 @@
         <v>Yellow</v>
       </c>
       <c r="F14" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="G14" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="G14" s="39" t="s">
+      <c r="H14" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="H14" s="39" t="s">
+      <c r="I14" s="41" t="s">
         <v>129</v>
       </c>
-      <c r="I14" s="41" t="s">
+      <c r="J14" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="J14" s="39" t="s">
-        <v>131</v>
-      </c>
       <c r="K14" s="71" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L14" s="68" t="s">
         <v>1</v>
       </c>
       <c r="M14" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="N14" s="75"/>
+        <v>131</v>
+      </c>
+      <c r="N14" s="73"/>
     </row>
     <row r="15" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A15" s="11"/>
@@ -3432,19 +3476,19 @@
         <v>Red</v>
       </c>
       <c r="F15" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="G15" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="G15" s="39" t="s">
+      <c r="H15" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="H15" s="39" t="s">
+      <c r="I15" s="41" t="s">
         <v>135</v>
       </c>
-      <c r="I15" s="41" t="s">
+      <c r="J15" s="39" t="s">
         <v>136</v>
-      </c>
-      <c r="J15" s="39" t="s">
-        <v>137</v>
       </c>
       <c r="K15" s="71" t="s">
         <v>68</v>
@@ -3453,9 +3497,9 @@
         <v>2</v>
       </c>
       <c r="M15" s="44" t="s">
-        <v>138</v>
-      </c>
-      <c r="N15" s="75"/>
+        <v>137</v>
+      </c>
+      <c r="N15" s="73"/>
     </row>
     <row r="16" spans="1:15" ht="36" x14ac:dyDescent="0.15">
       <c r="A16" s="11"/>
@@ -3473,30 +3517,30 @@
         <v>Yellow</v>
       </c>
       <c r="F16" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="G16" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="G16" s="39" t="s">
+      <c r="H16" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="H16" s="39" t="s">
+      <c r="I16" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="I16" s="41" t="s">
+      <c r="J16" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="J16" s="39" t="s">
-        <v>143</v>
-      </c>
       <c r="K16" s="71" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L16" s="68" t="s">
         <v>2</v>
       </c>
       <c r="M16" s="44" t="s">
-        <v>144</v>
-      </c>
-      <c r="N16" s="75"/>
+        <v>143</v>
+      </c>
+      <c r="N16" s="73"/>
     </row>
     <row r="17" spans="1:14" ht="60" x14ac:dyDescent="0.15">
       <c r="A17" s="11"/>
@@ -3514,49 +3558,71 @@
         <v>Red</v>
       </c>
       <c r="F17" s="42" t="s">
+        <v>144</v>
+      </c>
+      <c r="G17" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="G17" s="39" t="s">
+      <c r="H17" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="H17" s="39" t="s">
+      <c r="I17" s="41" t="s">
         <v>147</v>
       </c>
-      <c r="I17" s="41" t="s">
+      <c r="J17" s="39" t="s">
         <v>148</v>
       </c>
-      <c r="J17" s="39" t="s">
-        <v>149</v>
-      </c>
       <c r="K17" s="71" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L17" s="68" t="s">
         <v>1</v>
       </c>
       <c r="M17" s="44" t="s">
-        <v>150</v>
-      </c>
-      <c r="N17" s="75"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
+        <v>149</v>
+      </c>
+      <c r="N17" s="73"/>
+    </row>
+    <row r="18" spans="1:14" ht="36" x14ac:dyDescent="0.15">
       <c r="A18" s="11"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
+      <c r="B18" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>1</v>
+      </c>
       <c r="E18" s="63" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F18" s="42"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="71"/>
-      <c r="L18" s="68"/>
-      <c r="M18" s="44"/>
-      <c r="N18" s="75"/>
+        <v>Red</v>
+      </c>
+      <c r="F18" s="78" t="s">
+        <v>151</v>
+      </c>
+      <c r="G18" s="79" t="s">
+        <v>152</v>
+      </c>
+      <c r="H18" s="79" t="s">
+        <v>153</v>
+      </c>
+      <c r="I18" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="J18" s="79" t="s">
+        <v>155</v>
+      </c>
+      <c r="K18" s="71" t="s">
+        <v>116</v>
+      </c>
+      <c r="L18" s="68" t="s">
+        <v>1</v>
+      </c>
+      <c r="M18" s="81" t="s">
+        <v>156</v>
+      </c>
+      <c r="N18" s="73"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A19" s="11"/>
@@ -3575,7 +3641,7 @@
       <c r="K19" s="71"/>
       <c r="L19" s="68"/>
       <c r="M19" s="44"/>
-      <c r="N19" s="75"/>
+      <c r="N19" s="73"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A20" s="11"/>
@@ -3594,7 +3660,7 @@
       <c r="K20" s="71"/>
       <c r="L20" s="68"/>
       <c r="M20" s="44"/>
-      <c r="N20" s="75"/>
+      <c r="N20" s="73"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A21" s="11"/>
@@ -3613,7 +3679,7 @@
       <c r="K21" s="71"/>
       <c r="L21" s="68"/>
       <c r="M21" s="44"/>
-      <c r="N21" s="75"/>
+      <c r="N21" s="73"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A22" s="11"/>
@@ -3632,7 +3698,7 @@
       <c r="K22" s="71"/>
       <c r="L22" s="68"/>
       <c r="M22" s="44"/>
-      <c r="N22" s="75"/>
+      <c r="N22" s="73"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A23" s="11"/>
@@ -3651,7 +3717,7 @@
       <c r="K23" s="71"/>
       <c r="L23" s="68"/>
       <c r="M23" s="44"/>
-      <c r="N23" s="75"/>
+      <c r="N23" s="73"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A24" s="11"/>
@@ -3670,7 +3736,7 @@
       <c r="K24" s="71"/>
       <c r="L24" s="68"/>
       <c r="M24" s="44"/>
-      <c r="N24" s="75"/>
+      <c r="N24" s="73"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A25" s="11"/>
@@ -3689,7 +3755,7 @@
       <c r="K25" s="71"/>
       <c r="L25" s="68"/>
       <c r="M25" s="44"/>
-      <c r="N25" s="75"/>
+      <c r="N25" s="73"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A26" s="11"/>
@@ -3708,7 +3774,7 @@
       <c r="K26" s="71"/>
       <c r="L26" s="68"/>
       <c r="M26" s="44"/>
-      <c r="N26" s="75"/>
+      <c r="N26" s="73"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A27" s="11"/>
@@ -3727,7 +3793,7 @@
       <c r="K27" s="71"/>
       <c r="L27" s="68"/>
       <c r="M27" s="44"/>
-      <c r="N27" s="75"/>
+      <c r="N27" s="73"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A28" s="11"/>
@@ -3746,7 +3812,7 @@
       <c r="K28" s="71"/>
       <c r="L28" s="68"/>
       <c r="M28" s="44"/>
-      <c r="N28" s="75"/>
+      <c r="N28" s="73"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A29" s="11"/>
@@ -3765,7 +3831,7 @@
       <c r="K29" s="71"/>
       <c r="L29" s="68"/>
       <c r="M29" s="44"/>
-      <c r="N29" s="75"/>
+      <c r="N29" s="73"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A30" s="11"/>
@@ -3784,7 +3850,7 @@
       <c r="K30" s="71"/>
       <c r="L30" s="68"/>
       <c r="M30" s="44"/>
-      <c r="N30" s="75"/>
+      <c r="N30" s="73"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A31" s="11"/>
@@ -3803,7 +3869,7 @@
       <c r="K31" s="71"/>
       <c r="L31" s="68"/>
       <c r="M31" s="44"/>
-      <c r="N31" s="75"/>
+      <c r="N31" s="73"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A32" s="11"/>
@@ -3822,7 +3888,7 @@
       <c r="K32" s="71"/>
       <c r="L32" s="68"/>
       <c r="M32" s="44"/>
-      <c r="N32" s="75"/>
+      <c r="N32" s="73"/>
     </row>
     <row r="33" spans="1:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A33" s="12"/>
@@ -3837,310 +3903,310 @@
       <c r="G33" s="60"/>
       <c r="H33" s="60"/>
       <c r="I33" s="45"/>
-      <c r="J33" s="76"/>
+      <c r="J33" s="74"/>
       <c r="K33" s="67"/>
       <c r="L33" s="70"/>
       <c r="M33" s="46"/>
-      <c r="N33" s="75"/>
+      <c r="N33" s="73"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N34" s="75"/>
+      <c r="N34" s="73"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N35" s="75"/>
+      <c r="N35" s="73"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N36" s="75"/>
+      <c r="N36" s="73"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N37" s="75"/>
+      <c r="N37" s="73"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N38" s="75"/>
+      <c r="N38" s="73"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N39" s="75"/>
+      <c r="N39" s="73"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N40" s="75"/>
+      <c r="N40" s="73"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N41" s="75"/>
+      <c r="N41" s="73"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N42" s="75"/>
+      <c r="N42" s="73"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N43" s="75"/>
+      <c r="N43" s="73"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N44" s="75"/>
+      <c r="N44" s="73"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N45" s="75"/>
+      <c r="N45" s="73"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N46" s="75"/>
+      <c r="N46" s="73"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N47" s="75"/>
+      <c r="N47" s="73"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N48" s="75"/>
+      <c r="N48" s="73"/>
     </row>
     <row r="49" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N49" s="75"/>
+      <c r="N49" s="73"/>
     </row>
     <row r="50" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N50" s="75"/>
+      <c r="N50" s="73"/>
     </row>
     <row r="51" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N51" s="75"/>
+      <c r="N51" s="73"/>
     </row>
     <row r="52" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N52" s="75"/>
+      <c r="N52" s="73"/>
     </row>
     <row r="53" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N53" s="75"/>
+      <c r="N53" s="73"/>
     </row>
     <row r="54" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N54" s="75"/>
+      <c r="N54" s="73"/>
     </row>
     <row r="55" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N55" s="75"/>
+      <c r="N55" s="73"/>
     </row>
     <row r="56" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N56" s="75"/>
+      <c r="N56" s="73"/>
     </row>
     <row r="57" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N57" s="75"/>
+      <c r="N57" s="73"/>
     </row>
     <row r="58" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N58" s="75"/>
+      <c r="N58" s="73"/>
     </row>
     <row r="59" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N59" s="75"/>
+      <c r="N59" s="73"/>
     </row>
     <row r="60" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N60" s="75"/>
+      <c r="N60" s="73"/>
     </row>
     <row r="61" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N61" s="75"/>
+      <c r="N61" s="73"/>
     </row>
     <row r="62" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N62" s="75"/>
+      <c r="N62" s="73"/>
     </row>
     <row r="63" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N63" s="75"/>
+      <c r="N63" s="73"/>
     </row>
     <row r="64" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N64" s="75"/>
+      <c r="N64" s="73"/>
     </row>
     <row r="65" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N65" s="75"/>
+      <c r="N65" s="73"/>
     </row>
     <row r="66" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N66" s="75"/>
+      <c r="N66" s="73"/>
     </row>
     <row r="67" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N67" s="75"/>
+      <c r="N67" s="73"/>
     </row>
     <row r="68" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N68" s="75"/>
+      <c r="N68" s="73"/>
     </row>
     <row r="69" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N69" s="75"/>
+      <c r="N69" s="73"/>
     </row>
     <row r="70" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N70" s="75"/>
+      <c r="N70" s="73"/>
     </row>
     <row r="71" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N71" s="75"/>
+      <c r="N71" s="73"/>
     </row>
     <row r="72" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N72" s="75"/>
+      <c r="N72" s="73"/>
     </row>
     <row r="73" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N73" s="75"/>
+      <c r="N73" s="73"/>
     </row>
     <row r="74" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N74" s="75"/>
+      <c r="N74" s="73"/>
     </row>
     <row r="75" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N75" s="75"/>
+      <c r="N75" s="73"/>
     </row>
     <row r="76" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N76" s="75"/>
+      <c r="N76" s="73"/>
     </row>
     <row r="77" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N77" s="75"/>
+      <c r="N77" s="73"/>
     </row>
     <row r="78" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N78" s="75"/>
+      <c r="N78" s="73"/>
     </row>
     <row r="79" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N79" s="75"/>
+      <c r="N79" s="73"/>
     </row>
     <row r="80" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N80" s="75"/>
+      <c r="N80" s="73"/>
     </row>
     <row r="81" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N81" s="75"/>
+      <c r="N81" s="73"/>
     </row>
     <row r="82" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N82" s="75"/>
+      <c r="N82" s="73"/>
     </row>
     <row r="83" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N83" s="75"/>
+      <c r="N83" s="73"/>
     </row>
     <row r="84" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N84" s="75"/>
+      <c r="N84" s="73"/>
     </row>
     <row r="85" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N85" s="75"/>
+      <c r="N85" s="73"/>
     </row>
     <row r="86" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N86" s="75"/>
+      <c r="N86" s="73"/>
     </row>
     <row r="87" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N87" s="75"/>
+      <c r="N87" s="73"/>
     </row>
     <row r="88" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N88" s="75"/>
+      <c r="N88" s="73"/>
     </row>
     <row r="89" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N89" s="75"/>
+      <c r="N89" s="73"/>
     </row>
     <row r="90" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N90" s="75"/>
+      <c r="N90" s="73"/>
     </row>
     <row r="91" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N91" s="75"/>
+      <c r="N91" s="73"/>
     </row>
     <row r="92" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N92" s="75"/>
+      <c r="N92" s="73"/>
     </row>
     <row r="93" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N93" s="75"/>
+      <c r="N93" s="73"/>
     </row>
     <row r="94" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N94" s="75"/>
+      <c r="N94" s="73"/>
     </row>
     <row r="95" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N95" s="75"/>
+      <c r="N95" s="73"/>
     </row>
     <row r="96" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N96" s="75"/>
+      <c r="N96" s="73"/>
     </row>
     <row r="97" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N97" s="75"/>
+      <c r="N97" s="73"/>
     </row>
     <row r="98" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N98" s="75"/>
+      <c r="N98" s="73"/>
     </row>
     <row r="99" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N99" s="75"/>
+      <c r="N99" s="73"/>
     </row>
     <row r="100" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N100" s="75"/>
+      <c r="N100" s="73"/>
     </row>
     <row r="101" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N101" s="75"/>
+      <c r="N101" s="73"/>
     </row>
     <row r="102" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N102" s="75"/>
+      <c r="N102" s="73"/>
     </row>
     <row r="103" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N103" s="75"/>
+      <c r="N103" s="73"/>
     </row>
     <row r="104" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N104" s="75"/>
+      <c r="N104" s="73"/>
     </row>
     <row r="105" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N105" s="75"/>
+      <c r="N105" s="73"/>
     </row>
     <row r="106" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N106" s="75"/>
+      <c r="N106" s="73"/>
     </row>
     <row r="107" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N107" s="75"/>
+      <c r="N107" s="73"/>
     </row>
     <row r="108" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N108" s="75"/>
+      <c r="N108" s="73"/>
     </row>
     <row r="109" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N109" s="75"/>
+      <c r="N109" s="73"/>
     </row>
     <row r="110" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N110" s="75"/>
+      <c r="N110" s="73"/>
     </row>
     <row r="111" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N111" s="75"/>
+      <c r="N111" s="73"/>
     </row>
     <row r="112" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N112" s="75"/>
+      <c r="N112" s="73"/>
     </row>
     <row r="113" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N113" s="75"/>
+      <c r="N113" s="73"/>
     </row>
     <row r="114" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N114" s="75"/>
+      <c r="N114" s="73"/>
     </row>
     <row r="115" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N115" s="75"/>
+      <c r="N115" s="73"/>
     </row>
     <row r="116" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N116" s="75"/>
+      <c r="N116" s="73"/>
     </row>
     <row r="117" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N117" s="75"/>
+      <c r="N117" s="73"/>
     </row>
     <row r="118" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N118" s="75"/>
+      <c r="N118" s="73"/>
     </row>
     <row r="119" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N119" s="75"/>
+      <c r="N119" s="73"/>
     </row>
     <row r="120" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N120" s="75"/>
+      <c r="N120" s="73"/>
     </row>
     <row r="121" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N121" s="75"/>
+      <c r="N121" s="73"/>
     </row>
     <row r="122" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N122" s="75"/>
+      <c r="N122" s="73"/>
     </row>
     <row r="123" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N123" s="75"/>
+      <c r="N123" s="73"/>
     </row>
     <row r="124" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N124" s="75"/>
+      <c r="N124" s="73"/>
     </row>
     <row r="125" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N125" s="75"/>
+      <c r="N125" s="73"/>
     </row>
     <row r="126" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N126" s="75"/>
+      <c r="N126" s="73"/>
     </row>
     <row r="127" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N127" s="75"/>
+      <c r="N127" s="73"/>
     </row>
     <row r="128" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N128" s="75"/>
+      <c r="N128" s="73"/>
     </row>
     <row r="129" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N129" s="75"/>
+      <c r="N129" s="73"/>
     </row>
     <row r="130" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N130" s="75"/>
+      <c r="N130" s="73"/>
     </row>
     <row r="131" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N131" s="75"/>
+      <c r="N131" s="73"/>
     </row>
   </sheetData>
   <autoFilter ref="B6:D6" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="B6:C6 C1:E1 C34:E65534 B7:B33">
+  <conditionalFormatting sqref="B7:B33 B6:C6 C1:E1 C34:E65534">
     <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
@@ -4152,22 +4218,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:D33">
-    <cfRule type="cellIs" dxfId="7" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"High"</formula>
+    <cfRule type="cellIs" dxfId="7" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Low"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Low"</formula>
+    <cfRule type="cellIs" dxfId="5" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E33">
-    <cfRule type="cellIs" dxfId="4" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Yellow"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Red"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Yellow"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Green"</formula>

</xml_diff>

<commit_message>
Added to risk list 1.2 and 1.2.
</commit_message>
<xml_diff>
--- a/LCOM Documents/Iteration2/LCOMRiskList.xlsx
+++ b/LCOM Documents/Iteration2/LCOMRiskList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deepakchand/Desktop/ITC303-9-Team1-Project/LCOM Documents/Iteration2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4F6160-4210-7D4D-90D2-B0AE565D133A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5BB6D7-8075-A645-9D53-D99F79971A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -607,7 +607,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="164">
   <si>
     <t>ID</t>
   </si>
@@ -1423,9 +1423,6 @@
     <t>Apps accuracy is paramount for users.</t>
   </si>
   <si>
-    <t>Surety Considerations                         data/information                                    ds</t>
-  </si>
-  <si>
     <t>Tests show inaccurate outcomes.</t>
   </si>
   <si>
@@ -1439,6 +1436,24 @@
   </si>
   <si>
     <t>Just use local storage on device.</t>
+  </si>
+  <si>
+    <t>Usability risks</t>
+  </si>
+  <si>
+    <t>Simple usability and navigation  is important</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surety Considerations                         data/information                                   </t>
+  </si>
+  <si>
+    <t>App is difficult to navigate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If a week before Iteration 2.1, there are issues with usability and navigation, refer to contigency plan. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep app as simple as possible. </t>
   </si>
 </sst>
 </file>
@@ -2053,7 +2068,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2291,6 +2306,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2765,7 +2783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="222" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -2957,9 +2975,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3286,13 +3304,13 @@
         <v>104</v>
       </c>
       <c r="K10" s="71" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L10" s="68" t="s">
         <v>2</v>
       </c>
       <c r="M10" s="81" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N10" s="73"/>
     </row>
@@ -3563,7 +3581,7 @@
       <c r="G17" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="H17" s="39" t="s">
+      <c r="H17" s="79" t="s">
         <v>146</v>
       </c>
       <c r="I17" s="41" t="s">
@@ -3583,7 +3601,7 @@
       </c>
       <c r="N17" s="73"/>
     </row>
-    <row r="18" spans="1:14" ht="36" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:14" ht="24" x14ac:dyDescent="0.15">
       <c r="A18" s="11"/>
       <c r="B18" s="13" t="s">
         <v>8</v>
@@ -3605,13 +3623,13 @@
         <v>152</v>
       </c>
       <c r="H18" s="79" t="s">
+        <v>160</v>
+      </c>
+      <c r="I18" s="80" t="s">
         <v>153</v>
       </c>
-      <c r="I18" s="80" t="s">
+      <c r="J18" s="79" t="s">
         <v>154</v>
-      </c>
-      <c r="J18" s="79" t="s">
-        <v>155</v>
       </c>
       <c r="K18" s="71" t="s">
         <v>116</v>
@@ -3620,27 +3638,49 @@
         <v>1</v>
       </c>
       <c r="M18" s="81" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N18" s="73"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:14" ht="60" x14ac:dyDescent="0.15">
       <c r="A19" s="11"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
+      <c r="B19" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>1</v>
+      </c>
       <c r="E19" s="63" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F19" s="42"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="71"/>
-      <c r="L19" s="68"/>
-      <c r="M19" s="44"/>
+        <v>Red</v>
+      </c>
+      <c r="F19" s="78" t="s">
+        <v>158</v>
+      </c>
+      <c r="G19" s="79" t="s">
+        <v>159</v>
+      </c>
+      <c r="H19" s="79" t="s">
+        <v>146</v>
+      </c>
+      <c r="I19" s="80" t="s">
+        <v>161</v>
+      </c>
+      <c r="J19" s="79" t="s">
+        <v>162</v>
+      </c>
+      <c r="K19" s="82" t="s">
+        <v>68</v>
+      </c>
+      <c r="L19" s="68" t="s">
+        <v>1</v>
+      </c>
+      <c r="M19" s="81" t="s">
+        <v>163</v>
+      </c>
       <c r="N19" s="73"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Risks grouped into generic and specific category
</commit_message>
<xml_diff>
--- a/LCOM Documents/Iteration2/LCOMRiskList.xlsx
+++ b/LCOM Documents/Iteration2/LCOMRiskList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deepakchand/Desktop/ITC303-9-Team1-Project/LCOM Documents/Iteration2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41CD748-D5CA-034A-B818-D42D74A16BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060040F4-12CC-5B41-9510-CC0062ED0C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -607,7 +607,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="172">
   <si>
     <t>ID</t>
   </si>
@@ -1279,15 +1279,9 @@
     <t>A week prior to dealine, this will be dropped/ not pursued.</t>
   </si>
   <si>
-    <t>Makign the app attractive aesthetically to keep user motivated</t>
-  </si>
-  <si>
     <t>Requires skills beyond subject studied thus far: cybersecurity</t>
   </si>
   <si>
-    <t>If core use cases are not implemented, it would be hard to stay on track.</t>
-  </si>
-  <si>
     <t>Feasibility                                                Project resources</t>
   </si>
   <si>
@@ -1297,9 +1291,6 @@
     <t>Core use cases are unaccounted for.</t>
   </si>
   <si>
-    <t xml:space="preserve">Drop non-core usecases. </t>
-  </si>
-  <si>
     <t>Compatibility issues with different IDEs</t>
   </si>
   <si>
@@ -1315,9 +1306,6 @@
     <t>Contingency</t>
   </si>
   <si>
-    <t xml:space="preserve">High level of customisation such as font colour. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Such features may add additional difficulties. </t>
   </si>
   <si>
@@ -1472,6 +1460,24 @@
   </si>
   <si>
     <t xml:space="preserve">Functional inaccuracy </t>
+  </si>
+  <si>
+    <t>Not makign the app attractive aesthetically to keep user motivated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A dull looking home/activity page can cause user dissatisfaction and cause demotivation. </t>
+  </si>
+  <si>
+    <t>Drop non-core usecases such as requiring internet connection.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High level of customisation such as font colour and size. </t>
+  </si>
+  <si>
+    <t>APP Generic risks</t>
+  </si>
+  <si>
+    <t>APP Specific Risks</t>
   </si>
 </sst>
 </file>
@@ -1481,7 +1487,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1584,6 +1590,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1611,7 +1629,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -2082,11 +2100,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2114,9 +2169,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2330,6 +2382,24 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2360,6 +2430,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor indexed="45"/>
         </patternFill>
       </fill>
@@ -2374,6 +2451,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor indexed="45"/>
         </patternFill>
       </fill>
@@ -2381,21 +2465,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2810,173 +2880,173 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="93" style="9" customWidth="1"/>
     <col min="3" max="16384" width="9.1640625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="str">
+      <c r="A1" s="81" t="str">
         <f>Risk_Tracking_Log!A1</f>
         <v>RISK MANAGEMENT LOG</v>
       </c>
-      <c r="B1" s="83"/>
+      <c r="B1" s="82"/>
     </row>
     <row r="2" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12" x14ac:dyDescent="0.15">
-      <c r="A3" s="21"/>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="20"/>
+      <c r="B3" s="14" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12" x14ac:dyDescent="0.15">
-      <c r="A4" s="19"/>
-      <c r="B4" s="16" t="s">
+      <c r="A4" s="18"/>
+      <c r="B4" s="15" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12" x14ac:dyDescent="0.15">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="47" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="48" x14ac:dyDescent="0.15">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="47" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="72" x14ac:dyDescent="0.15">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="47" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="12" x14ac:dyDescent="0.15">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="48" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.15">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="47" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="12" x14ac:dyDescent="0.15">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="47" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="12" x14ac:dyDescent="0.15">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="47" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="12" x14ac:dyDescent="0.15">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="47" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="12" x14ac:dyDescent="0.15">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="47" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12" x14ac:dyDescent="0.15">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="47" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="12" x14ac:dyDescent="0.15">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="47" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="12" x14ac:dyDescent="0.15">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="47" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="65" t="s">
+      <c r="A17" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="65" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="37" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="21" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="17" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="61" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="21" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2997,8 +3067,8 @@
   <dimension ref="A1:O131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3008,11 +3078,11 @@
     <col min="3" max="3" width="10.5" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="34" style="47" customWidth="1"/>
-    <col min="8" max="8" width="22.1640625" style="47" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="30.83203125" style="47" customWidth="1"/>
-    <col min="11" max="11" width="12.83203125" style="47" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="30.83203125" style="47" customWidth="1"/>
+    <col min="6" max="7" width="34" style="46" customWidth="1"/>
+    <col min="8" max="8" width="22.1640625" style="46" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="30.83203125" style="46" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" style="46" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="30.83203125" style="46" customWidth="1"/>
     <col min="15" max="15" width="6" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3020,193 +3090,195 @@
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
       <c r="I1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
       <c r="I2" s="7" t="str">
         <f>A2</f>
         <v>Project Name:</v>
       </c>
-      <c r="J2" s="30" t="str">
+      <c r="J2" s="29" t="str">
         <f>D2</f>
         <v>ADHD Task Manager</v>
       </c>
-      <c r="K2" s="36"/>
+      <c r="K2" s="35"/>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3" s="35"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
       <c r="I3" s="8" t="str">
         <f>A3</f>
         <v>National Center:</v>
       </c>
-      <c r="J3" s="34" t="str">
+      <c r="J3" s="33" t="str">
         <f>D3</f>
         <v>Australia</v>
       </c>
-      <c r="K3" s="36"/>
+      <c r="K3" s="35"/>
     </row>
     <row r="4" spans="1:15" s="1" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="37" t="s">
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
       <c r="I4" s="8" t="str">
         <f>A4</f>
         <v>Project Manager Name:</v>
       </c>
-      <c r="J4" s="37" t="str">
+      <c r="J4" s="36" t="str">
         <f>D4</f>
         <v>Team 1</v>
       </c>
-      <c r="K4" s="36"/>
+      <c r="K4" s="35"/>
     </row>
     <row r="5" spans="1:15" s="1" customFormat="1" ht="61" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="75" t="s">
-        <v>149</v>
-      </c>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="74" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
       <c r="I5" s="8" t="str">
         <f>A5</f>
         <v>Project Description:</v>
       </c>
-      <c r="J5" s="50" t="str">
+      <c r="J5" s="49" t="str">
         <f>D5</f>
         <v>Task Manager app for individuals with ADHD to complete tasks, gain rewards, and stay motivated.</v>
       </c>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="52"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="51"/>
     </row>
     <row r="6" spans="1:15" s="3" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="53" t="s">
+      <c r="D6" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="53" t="s">
+      <c r="E6" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="55" t="s">
+      <c r="F6" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="55" t="s">
+      <c r="G6" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="58" t="s">
+      <c r="H6" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="53" t="s">
+      <c r="I6" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="53" t="s">
+      <c r="J6" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="K6" s="53" t="s">
+      <c r="K6" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="55" t="s">
+      <c r="L6" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="M6" s="64" t="s">
+      <c r="M6" s="63" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="111" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="10"/>
-      <c r="B7" s="13" t="s">
+      <c r="A7" s="83" t="s">
+        <v>170</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="63" t="str">
+      <c r="E7" s="62" t="str">
         <f>IF(OR(AND(B7&lt;&gt;"Closed",C7="High",D7="High"),AND(B7&lt;&gt;"Closed",C7="High",D7="Medium"),AND(B7&lt;&gt;"Closed",C7="Medium",D7="High")),"Red",IF(OR(AND(B7&lt;&gt;"Closed",C7="High",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Medium",D7="Medium"),AND(B7&lt;&gt;"Closed",C7="Low",D7="High")),"Yellow",IF(OR(AND(B7&lt;&gt;"Closed",C7="Medium",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Low",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Low",D7="Medium")),"Green",IF(B7="Closed","Closed",""))))</f>
         <v>Yellow</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="G7" s="40" t="s">
+      <c r="G7" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="H7" s="39" t="s">
+      <c r="H7" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="I7" s="40" t="s">
+      <c r="I7" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="J7" s="40" t="s">
+      <c r="J7" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="K7" s="71" t="s">
+      <c r="K7" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="L7" s="40" t="s">
+      <c r="L7" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="M7" s="62" t="s">
+      <c r="M7" s="61" t="s">
         <v>80</v>
       </c>
       <c r="O7" t="str">
@@ -3215,1108 +3287,1114 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="53" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="10"/>
-      <c r="B8" s="13" t="s">
+      <c r="A8" s="84"/>
+      <c r="B8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="63" t="str">
+      <c r="E8" s="62" t="str">
         <f t="shared" ref="E8:E33" si="0">IF(OR(AND(B8&lt;&gt;"Closed",C8="High",D8="High"),AND(B8&lt;&gt;"Closed",C8="High",D8="Medium"),AND(B8&lt;&gt;"Closed",C8="Medium",D8="High")),"Red",IF(OR(AND(B8&lt;&gt;"Closed",C8="High",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Medium",D8="Medium"),AND(B8&lt;&gt;"Closed",C8="Low",D8="High")),"Yellow",IF(OR(AND(B8&lt;&gt;"Closed",C8="Medium",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Low",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Low",D8="Medium")),"Green",IF(B8="Closed","Closed",""))))</f>
         <v>Yellow</v>
       </c>
-      <c r="F8" s="42" t="s">
+      <c r="F8" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="G8" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="I8" s="41" t="s">
+      <c r="I8" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="J8" s="39" t="s">
+      <c r="J8" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="K8" s="71" t="s">
+      <c r="K8" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="L8" s="68" t="s">
+      <c r="L8" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="M8" s="44" t="s">
+      <c r="M8" s="43" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="A9" s="10"/>
-      <c r="B9" s="13" t="s">
+      <c r="A9" s="84"/>
+      <c r="B9" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="61" t="s">
+      <c r="D9" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="63" t="str">
+      <c r="E9" s="62" t="str">
         <f t="shared" si="0"/>
         <v>Closed</v>
       </c>
-      <c r="F9" s="41" t="s">
+      <c r="F9" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G9" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="H9" s="39" t="s">
+      <c r="H9" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="I9" s="41" t="s">
+      <c r="I9" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="J9" s="39" t="s">
+      <c r="J9" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="K9" s="71" t="s">
+      <c r="K9" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="L9" s="69" t="s">
+      <c r="L9" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="M9" s="43" t="s">
+      <c r="M9" s="42" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="36" x14ac:dyDescent="0.15">
-      <c r="A10" s="11"/>
-      <c r="B10" s="13" t="s">
+    <row r="10" spans="1:15" ht="48" x14ac:dyDescent="0.15">
+      <c r="A10" s="84"/>
+      <c r="B10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="62" t="str">
+        <f>IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="High"),AND(B10&lt;&gt;"Closed",C10="High",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="High")),"Red",IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Low",D10="High")),"Yellow",IF(OR(AND(B10&lt;&gt;"Closed",C10="Medium",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Medium")),"Green",IF(B10="Closed","Closed",""))))</f>
+        <v>Red</v>
+      </c>
+      <c r="F10" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="G10" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="H10" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="I10" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="J10" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="K10" s="70" t="s">
+        <v>113</v>
+      </c>
+      <c r="L10" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="M10" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="N10" s="72"/>
+    </row>
+    <row r="11" spans="1:15" ht="60" x14ac:dyDescent="0.15">
+      <c r="A11" s="84"/>
+      <c r="B11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="62" t="str">
+        <f>IF(OR(AND(B11&lt;&gt;"Closed",C11="High",D11="High"),AND(B11&lt;&gt;"Closed",C11="High",D11="Medium"),AND(B11&lt;&gt;"Closed",C11="Medium",D11="High")),"Red",IF(OR(AND(B11&lt;&gt;"Closed",C11="High",D11="Low"),AND(B11&lt;&gt;"Closed",C11="Medium",D11="Medium"),AND(B11&lt;&gt;"Closed",C11="Low",D11="High")),"Yellow",IF(OR(AND(B11&lt;&gt;"Closed",C11="Medium",D11="Low"),AND(B11&lt;&gt;"Closed",C11="Low",D11="Low"),AND(B11&lt;&gt;"Closed",C11="Low",D11="Medium")),"Green",IF(B11="Closed","Closed",""))))</f>
+        <v>Red</v>
+      </c>
+      <c r="F11" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="H11" s="76" t="s">
+        <v>141</v>
+      </c>
+      <c r="I11" s="40" t="s">
+        <v>142</v>
+      </c>
+      <c r="J11" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="K11" s="70" t="s">
+        <v>113</v>
+      </c>
+      <c r="L11" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="N11" s="72"/>
+    </row>
+    <row r="12" spans="1:15" ht="24" x14ac:dyDescent="0.15">
+      <c r="A12" s="84"/>
+      <c r="B12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="63" t="str">
+      <c r="E12" s="62" t="str">
+        <f>IF(OR(AND(B12&lt;&gt;"Closed",C12="High",D12="High"),AND(B12&lt;&gt;"Closed",C12="High",D12="Medium"),AND(B12&lt;&gt;"Closed",C12="Medium",D12="High")),"Red",IF(OR(AND(B12&lt;&gt;"Closed",C12="High",D12="Low"),AND(B12&lt;&gt;"Closed",C12="Medium",D12="Medium"),AND(B12&lt;&gt;"Closed",C12="Low",D12="High")),"Yellow",IF(OR(AND(B12&lt;&gt;"Closed",C12="Medium",D12="Low"),AND(B12&lt;&gt;"Closed",C12="Low",D12="Low"),AND(B12&lt;&gt;"Closed",C12="Low",D12="Medium")),"Green",IF(B12="Closed","Closed",""))))</f>
+        <v>Red</v>
+      </c>
+      <c r="F12" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="H12" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="I12" s="77" t="s">
+        <v>164</v>
+      </c>
+      <c r="J12" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="K12" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="L12" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="M12" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="N12" s="72"/>
+    </row>
+    <row r="13" spans="1:15" ht="36" x14ac:dyDescent="0.15">
+      <c r="A13" s="85"/>
+      <c r="B13" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="62" t="str">
+        <f>IF(OR(AND(B13&lt;&gt;"Closed",C13="High",D13="High"),AND(B13&lt;&gt;"Closed",C13="High",D13="Medium"),AND(B13&lt;&gt;"Closed",C13="Medium",D13="High")),"Red",IF(OR(AND(B13&lt;&gt;"Closed",C13="High",D13="Low"),AND(B13&lt;&gt;"Closed",C13="Medium",D13="Medium"),AND(B13&lt;&gt;"Closed",C13="Low",D13="High")),"Yellow",IF(OR(AND(B13&lt;&gt;"Closed",C13="Medium",D13="Low"),AND(B13&lt;&gt;"Closed",C13="Low",D13="Low"),AND(B13&lt;&gt;"Closed",C13="Low",D13="Medium")),"Green",IF(B13="Closed","Closed",""))))</f>
+        <v>Red</v>
+      </c>
+      <c r="F13" s="75" t="s">
+        <v>158</v>
+      </c>
+      <c r="G13" s="76" t="s">
+        <v>159</v>
+      </c>
+      <c r="H13" s="76" t="s">
+        <v>160</v>
+      </c>
+      <c r="I13" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="J13" s="76" t="s">
+        <v>162</v>
+      </c>
+      <c r="K13" s="79" t="s">
+        <v>113</v>
+      </c>
+      <c r="L13" s="80" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" s="78" t="s">
+        <v>163</v>
+      </c>
+      <c r="N13" s="72"/>
+    </row>
+    <row r="14" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="86" t="s">
+        <v>171</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="62" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
-      <c r="F10" s="42" t="s">
+      <c r="F14" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="G10" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="H10" s="39" t="s">
+      <c r="G14" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="H14" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="I10" s="41" t="s">
+      <c r="I14" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="J10" s="39" t="s">
+      <c r="J14" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="K10" s="71" t="s">
-        <v>154</v>
-      </c>
-      <c r="L10" s="68" t="s">
+      <c r="K14" s="70" t="s">
+        <v>150</v>
+      </c>
+      <c r="L14" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="M10" s="79" t="s">
+      <c r="M14" s="78" t="s">
+        <v>151</v>
+      </c>
+      <c r="N14" s="72"/>
+    </row>
+    <row r="15" spans="1:15" ht="36" x14ac:dyDescent="0.15">
+      <c r="A15" s="87"/>
+      <c r="B15" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>Yellow</v>
+      </c>
+      <c r="F15" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="G15" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="H15" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="I15" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="J15" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="K15" s="70" t="s">
+        <v>113</v>
+      </c>
+      <c r="L15" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="M15" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="N15" s="72"/>
+    </row>
+    <row r="16" spans="1:15" ht="60" x14ac:dyDescent="0.15">
+      <c r="A16" s="87"/>
+      <c r="B16" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="62" t="str">
+        <f>IF(OR(AND(B16&lt;&gt;"Closed",C16="High",D16="High"),AND(B16&lt;&gt;"Closed",C16="High",D16="Medium"),AND(B16&lt;&gt;"Closed",C16="Medium",D16="High")),"Red",IF(OR(AND(B16&lt;&gt;"Closed",C16="High",D16="Low"),AND(B16&lt;&gt;"Closed",C16="Medium",D16="Medium"),AND(B16&lt;&gt;"Closed",C16="Low",D16="High")),"Yellow",IF(OR(AND(B16&lt;&gt;"Closed",C16="Medium",D16="Low"),AND(B16&lt;&gt;"Closed",C16="Low",D16="Low"),AND(B16&lt;&gt;"Closed",C16="Low",D16="Medium")),"Green",IF(B16="Closed","Closed",""))))</f>
+        <v>Red</v>
+      </c>
+      <c r="F16" s="75" t="s">
+        <v>152</v>
+      </c>
+      <c r="G16" s="76" t="s">
+        <v>153</v>
+      </c>
+      <c r="H16" s="76" t="s">
+        <v>141</v>
+      </c>
+      <c r="I16" s="77" t="s">
         <v>155</v>
       </c>
-      <c r="N10" s="73"/>
-    </row>
-    <row r="11" spans="1:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="A11" s="11"/>
-      <c r="B11" s="13" t="s">
+      <c r="J16" s="76" t="s">
+        <v>156</v>
+      </c>
+      <c r="K16" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="L16" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="M16" s="78" t="s">
+        <v>157</v>
+      </c>
+      <c r="N16" s="72"/>
+    </row>
+    <row r="17" spans="1:14" ht="36" x14ac:dyDescent="0.15">
+      <c r="A17" s="87"/>
+      <c r="B17" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C17" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="E17" s="62" t="str">
+        <f t="shared" si="0"/>
+        <v>Yellow</v>
+      </c>
+      <c r="F17" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="G17" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="H17" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="I17" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="J17" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="K17" s="70" t="s">
+        <v>113</v>
+      </c>
+      <c r="L17" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="63" t="str">
-        <f t="shared" si="0"/>
-        <v>Green</v>
-      </c>
-      <c r="F11" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="G11" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="H11" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="I11" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="J11" s="39" t="s">
-        <v>110</v>
-      </c>
-      <c r="K11" s="71" t="s">
-        <v>68</v>
-      </c>
-      <c r="L11" s="68" t="s">
-        <v>3</v>
-      </c>
-      <c r="M11" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="N11" s="73"/>
-    </row>
-    <row r="12" spans="1:15" ht="48" x14ac:dyDescent="0.15">
-      <c r="A12" s="11"/>
-      <c r="B12" s="13" t="s">
+      <c r="M17" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="N17" s="72"/>
+    </row>
+    <row r="18" spans="1:14" ht="24" x14ac:dyDescent="0.15">
+      <c r="A18" s="87"/>
+      <c r="B18" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C18" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D18" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="63" t="str">
+      <c r="E18" s="62" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
-      <c r="F12" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="G12" s="39" t="s">
+      <c r="F18" s="75" t="s">
+        <v>165</v>
+      </c>
+      <c r="G18" s="76" t="s">
+        <v>146</v>
+      </c>
+      <c r="H18" s="76" t="s">
+        <v>154</v>
+      </c>
+      <c r="I18" s="77" t="s">
+        <v>147</v>
+      </c>
+      <c r="J18" s="76" t="s">
+        <v>148</v>
+      </c>
+      <c r="K18" s="70" t="s">
         <v>113</v>
       </c>
-      <c r="H12" s="39" t="s">
+      <c r="L18" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="M18" s="78" t="s">
+        <v>149</v>
+      </c>
+      <c r="N18" s="72"/>
+    </row>
+    <row r="19" spans="1:14" ht="24" x14ac:dyDescent="0.15">
+      <c r="A19" s="87"/>
+      <c r="B19" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="62" t="str">
+        <f>IF(OR(AND(B19&lt;&gt;"Closed",C19="High",D19="High"),AND(B19&lt;&gt;"Closed",C19="High",D19="Medium"),AND(B19&lt;&gt;"Closed",C19="Medium",D19="High")),"Red",IF(OR(AND(B19&lt;&gt;"Closed",C19="High",D19="Low"),AND(B19&lt;&gt;"Closed",C19="Medium",D19="Medium"),AND(B19&lt;&gt;"Closed",C19="Low",D19="High")),"Yellow",IF(OR(AND(B19&lt;&gt;"Closed",C19="Medium",D19="Low"),AND(B19&lt;&gt;"Closed",C19="Low",D19="Low"),AND(B19&lt;&gt;"Closed",C19="Low",D19="Medium")),"Green",IF(B19="Closed","Closed",""))))</f>
+        <v>Green</v>
+      </c>
+      <c r="F19" s="75" t="s">
+        <v>166</v>
+      </c>
+      <c r="G19" s="76" t="s">
+        <v>167</v>
+      </c>
+      <c r="H19" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="I19" s="77" t="s">
+        <v>107</v>
+      </c>
+      <c r="J19" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="K19" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="L19" s="67" t="s">
+        <v>3</v>
+      </c>
+      <c r="M19" s="78" t="s">
+        <v>168</v>
+      </c>
+      <c r="N19" s="72"/>
+    </row>
+    <row r="20" spans="1:14" ht="24" x14ac:dyDescent="0.15">
+      <c r="A20" s="88"/>
+      <c r="B20" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="62" t="str">
+        <f>IF(OR(AND(B20&lt;&gt;"Closed",C20="High",D20="High"),AND(B20&lt;&gt;"Closed",C20="High",D20="Medium"),AND(B20&lt;&gt;"Closed",C20="Medium",D20="High")),"Red",IF(OR(AND(B20&lt;&gt;"Closed",C20="High",D20="Low"),AND(B20&lt;&gt;"Closed",C20="Medium",D20="Medium"),AND(B20&lt;&gt;"Closed",C20="Low",D20="High")),"Yellow",IF(OR(AND(B20&lt;&gt;"Closed",C20="Medium",D20="Low"),AND(B20&lt;&gt;"Closed",C20="Low",D20="Low"),AND(B20&lt;&gt;"Closed",C20="Low",D20="Medium")),"Green",IF(B20="Closed","Closed",""))))</f>
+        <v>Yellow</v>
+      </c>
+      <c r="F20" s="75" t="s">
+        <v>169</v>
+      </c>
+      <c r="G20" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="H20" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="J20" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="K20" s="70" t="s">
+        <v>119</v>
+      </c>
+      <c r="L20" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="M20" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="I12" s="41" t="s">
-        <v>114</v>
-      </c>
-      <c r="J12" s="39" t="s">
-        <v>115</v>
-      </c>
-      <c r="K12" s="71" t="s">
-        <v>116</v>
-      </c>
-      <c r="L12" s="68" t="s">
-        <v>1</v>
-      </c>
-      <c r="M12" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="N12" s="73"/>
-    </row>
-    <row r="13" spans="1:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="A13" s="11"/>
-      <c r="B13" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="63" t="str">
-        <f t="shared" si="0"/>
-        <v>Yellow</v>
-      </c>
-      <c r="F13" s="42" t="s">
-        <v>117</v>
-      </c>
-      <c r="G13" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="H13" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13" s="41" t="s">
-        <v>121</v>
-      </c>
-      <c r="J13" s="39" t="s">
-        <v>122</v>
-      </c>
-      <c r="K13" s="71" t="s">
-        <v>123</v>
-      </c>
-      <c r="L13" s="68" t="s">
-        <v>2</v>
-      </c>
-      <c r="M13" s="44" t="s">
-        <v>124</v>
-      </c>
-      <c r="N13" s="73"/>
-    </row>
-    <row r="14" spans="1:15" ht="36" x14ac:dyDescent="0.15">
-      <c r="A14" s="11"/>
-      <c r="B14" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="63" t="str">
-        <f t="shared" si="0"/>
-        <v>Yellow</v>
-      </c>
-      <c r="F14" s="42" t="s">
-        <v>126</v>
-      </c>
-      <c r="G14" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="H14" s="39" t="s">
-        <v>128</v>
-      </c>
-      <c r="I14" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="J14" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="K14" s="71" t="s">
-        <v>116</v>
-      </c>
-      <c r="L14" s="68" t="s">
-        <v>1</v>
-      </c>
-      <c r="M14" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="N14" s="73"/>
-    </row>
-    <row r="15" spans="1:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="A15" s="11"/>
-      <c r="B15" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="63" t="str">
-        <f t="shared" si="0"/>
-        <v>Red</v>
-      </c>
-      <c r="F15" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="G15" s="39" t="s">
-        <v>133</v>
-      </c>
-      <c r="H15" s="39" t="s">
-        <v>134</v>
-      </c>
-      <c r="I15" s="78" t="s">
-        <v>168</v>
-      </c>
-      <c r="J15" s="39" t="s">
-        <v>135</v>
-      </c>
-      <c r="K15" s="71" t="s">
-        <v>68</v>
-      </c>
-      <c r="L15" s="68" t="s">
-        <v>2</v>
-      </c>
-      <c r="M15" s="44" t="s">
-        <v>136</v>
-      </c>
-      <c r="N15" s="73"/>
-    </row>
-    <row r="16" spans="1:15" ht="36" x14ac:dyDescent="0.15">
-      <c r="A16" s="11"/>
-      <c r="B16" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="63" t="str">
-        <f t="shared" si="0"/>
-        <v>Yellow</v>
-      </c>
-      <c r="F16" s="42" t="s">
-        <v>137</v>
-      </c>
-      <c r="G16" s="39" t="s">
-        <v>138</v>
-      </c>
-      <c r="H16" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="I16" s="41" t="s">
-        <v>140</v>
-      </c>
-      <c r="J16" s="39" t="s">
-        <v>141</v>
-      </c>
-      <c r="K16" s="71" t="s">
-        <v>116</v>
-      </c>
-      <c r="L16" s="68" t="s">
-        <v>2</v>
-      </c>
-      <c r="M16" s="44" t="s">
-        <v>142</v>
-      </c>
-      <c r="N16" s="73"/>
-    </row>
-    <row r="17" spans="1:14" ht="60" x14ac:dyDescent="0.15">
-      <c r="A17" s="11"/>
-      <c r="B17" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="63" t="str">
-        <f t="shared" si="0"/>
-        <v>Red</v>
-      </c>
-      <c r="F17" s="42" t="s">
-        <v>143</v>
-      </c>
-      <c r="G17" s="39" t="s">
-        <v>144</v>
-      </c>
-      <c r="H17" s="77" t="s">
-        <v>145</v>
-      </c>
-      <c r="I17" s="41" t="s">
-        <v>146</v>
-      </c>
-      <c r="J17" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="K17" s="71" t="s">
-        <v>116</v>
-      </c>
-      <c r="L17" s="68" t="s">
-        <v>1</v>
-      </c>
-      <c r="M17" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="N17" s="73"/>
-    </row>
-    <row r="18" spans="1:14" ht="24" x14ac:dyDescent="0.15">
-      <c r="A18" s="11"/>
-      <c r="B18" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="63" t="str">
-        <f t="shared" si="0"/>
-        <v>Red</v>
-      </c>
-      <c r="F18" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="G18" s="77" t="s">
-        <v>150</v>
-      </c>
-      <c r="H18" s="77" t="s">
-        <v>158</v>
-      </c>
-      <c r="I18" s="78" t="s">
-        <v>151</v>
-      </c>
-      <c r="J18" s="77" t="s">
-        <v>152</v>
-      </c>
-      <c r="K18" s="71" t="s">
-        <v>116</v>
-      </c>
-      <c r="L18" s="68" t="s">
-        <v>1</v>
-      </c>
-      <c r="M18" s="79" t="s">
-        <v>153</v>
-      </c>
-      <c r="N18" s="73"/>
-    </row>
-    <row r="19" spans="1:14" ht="60" x14ac:dyDescent="0.15">
-      <c r="A19" s="11"/>
-      <c r="B19" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="63" t="str">
-        <f t="shared" si="0"/>
-        <v>Red</v>
-      </c>
-      <c r="F19" s="76" t="s">
-        <v>156</v>
-      </c>
-      <c r="G19" s="77" t="s">
-        <v>157</v>
-      </c>
-      <c r="H19" s="77" t="s">
-        <v>145</v>
-      </c>
-      <c r="I19" s="78" t="s">
-        <v>159</v>
-      </c>
-      <c r="J19" s="77" t="s">
-        <v>160</v>
-      </c>
-      <c r="K19" s="80" t="s">
-        <v>68</v>
-      </c>
-      <c r="L19" s="68" t="s">
-        <v>1</v>
-      </c>
-      <c r="M19" s="79" t="s">
-        <v>161</v>
-      </c>
-      <c r="N19" s="73"/>
-    </row>
-    <row r="20" spans="1:14" ht="36" x14ac:dyDescent="0.15">
-      <c r="A20" s="11"/>
-      <c r="B20" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" s="63" t="str">
-        <f t="shared" si="0"/>
-        <v>Red</v>
-      </c>
-      <c r="F20" s="76" t="s">
-        <v>162</v>
-      </c>
-      <c r="G20" s="77" t="s">
-        <v>163</v>
-      </c>
-      <c r="H20" s="77" t="s">
-        <v>164</v>
-      </c>
-      <c r="I20" s="78" t="s">
-        <v>165</v>
-      </c>
-      <c r="J20" s="77" t="s">
-        <v>166</v>
-      </c>
-      <c r="K20" s="80" t="s">
-        <v>116</v>
-      </c>
-      <c r="L20" s="81" t="s">
-        <v>2</v>
-      </c>
-      <c r="M20" s="79" t="s">
-        <v>167</v>
-      </c>
-      <c r="N20" s="73"/>
+      <c r="N20" s="72"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A21" s="11"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="63" t="str">
+      <c r="A21" s="10"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="62" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F21" s="42"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="71"/>
-      <c r="L21" s="68"/>
-      <c r="M21" s="44"/>
-      <c r="N21" s="73"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="70"/>
+      <c r="L21" s="67"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="72"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A22" s="11"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="63" t="str">
+      <c r="A22" s="10"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="62" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F22" s="42"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="71"/>
-      <c r="L22" s="68"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="73"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="70"/>
+      <c r="L22" s="67"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="72"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A23" s="11"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="63" t="str">
+      <c r="A23" s="10"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="62" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F23" s="42"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="41"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="71"/>
-      <c r="L23" s="68"/>
-      <c r="M23" s="44"/>
-      <c r="N23" s="73"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="70"/>
+      <c r="L23" s="67"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="72"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A24" s="11"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="63" t="str">
+      <c r="A24" s="10"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="62" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F24" s="42"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="71"/>
-      <c r="L24" s="68"/>
-      <c r="M24" s="44"/>
-      <c r="N24" s="73"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="70"/>
+      <c r="L24" s="67"/>
+      <c r="M24" s="43"/>
+      <c r="N24" s="72"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A25" s="11"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="63" t="str">
+      <c r="A25" s="10"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="62" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F25" s="42"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="39"/>
-      <c r="K25" s="71"/>
-      <c r="L25" s="68"/>
-      <c r="M25" s="44"/>
-      <c r="N25" s="73"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="70"/>
+      <c r="L25" s="67"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="72"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A26" s="11"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="63" t="str">
+      <c r="A26" s="10"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="62" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F26" s="42"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="39"/>
-      <c r="K26" s="71"/>
-      <c r="L26" s="68"/>
-      <c r="M26" s="44"/>
-      <c r="N26" s="73"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="70"/>
+      <c r="L26" s="67"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="72"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A27" s="11"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="63" t="str">
+      <c r="A27" s="10"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="62" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F27" s="42"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="41"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="71"/>
-      <c r="L27" s="68"/>
-      <c r="M27" s="44"/>
-      <c r="N27" s="73"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="70"/>
+      <c r="L27" s="67"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="72"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A28" s="11"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="63" t="str">
+      <c r="A28" s="10"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="62" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F28" s="42"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="71"/>
-      <c r="L28" s="68"/>
-      <c r="M28" s="44"/>
-      <c r="N28" s="73"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="70"/>
+      <c r="L28" s="67"/>
+      <c r="M28" s="43"/>
+      <c r="N28" s="72"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A29" s="11"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="63" t="str">
+      <c r="A29" s="10"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="62" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F29" s="42"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="41"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="71"/>
-      <c r="L29" s="68"/>
-      <c r="M29" s="44"/>
-      <c r="N29" s="73"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="70"/>
+      <c r="L29" s="67"/>
+      <c r="M29" s="43"/>
+      <c r="N29" s="72"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A30" s="11"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="63" t="str">
+      <c r="A30" s="10"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="62" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F30" s="42"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="39"/>
-      <c r="K30" s="71"/>
-      <c r="L30" s="68"/>
-      <c r="M30" s="44"/>
-      <c r="N30" s="73"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="70"/>
+      <c r="L30" s="67"/>
+      <c r="M30" s="43"/>
+      <c r="N30" s="72"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A31" s="11"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="63" t="str">
+      <c r="A31" s="10"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="62" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F31" s="42"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="41"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="71"/>
-      <c r="L31" s="68"/>
-      <c r="M31" s="44"/>
-      <c r="N31" s="73"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="70"/>
+      <c r="L31" s="67"/>
+      <c r="M31" s="43"/>
+      <c r="N31" s="72"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A32" s="11"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="63" t="str">
+      <c r="A32" s="10"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="62" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F32" s="42"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="41"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="71"/>
-      <c r="L32" s="68"/>
-      <c r="M32" s="44"/>
-      <c r="N32" s="73"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="38"/>
+      <c r="K32" s="70"/>
+      <c r="L32" s="67"/>
+      <c r="M32" s="43"/>
+      <c r="N32" s="72"/>
     </row>
     <row r="33" spans="1:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="12"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="59"/>
-      <c r="D33" s="59"/>
-      <c r="E33" s="14" t="str">
+      <c r="A33" s="11"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="13" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F33" s="45"/>
-      <c r="G33" s="60"/>
-      <c r="H33" s="60"/>
-      <c r="I33" s="45"/>
-      <c r="J33" s="74"/>
-      <c r="K33" s="67"/>
-      <c r="L33" s="70"/>
-      <c r="M33" s="46"/>
-      <c r="N33" s="73"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="73"/>
+      <c r="K33" s="66"/>
+      <c r="L33" s="69"/>
+      <c r="M33" s="45"/>
+      <c r="N33" s="72"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N34" s="73"/>
+      <c r="N34" s="72"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N35" s="73"/>
+      <c r="N35" s="72"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N36" s="73"/>
+      <c r="N36" s="72"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N37" s="73"/>
+      <c r="N37" s="72"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N38" s="73"/>
+      <c r="N38" s="72"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N39" s="73"/>
+      <c r="N39" s="72"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N40" s="73"/>
+      <c r="N40" s="72"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N41" s="73"/>
+      <c r="N41" s="72"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N42" s="73"/>
+      <c r="N42" s="72"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N43" s="73"/>
+      <c r="N43" s="72"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N44" s="73"/>
+      <c r="N44" s="72"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N45" s="73"/>
+      <c r="N45" s="72"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N46" s="73"/>
+      <c r="N46" s="72"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N47" s="73"/>
+      <c r="N47" s="72"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N48" s="73"/>
+      <c r="N48" s="72"/>
     </row>
     <row r="49" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N49" s="73"/>
+      <c r="N49" s="72"/>
     </row>
     <row r="50" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N50" s="73"/>
+      <c r="N50" s="72"/>
     </row>
     <row r="51" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N51" s="73"/>
+      <c r="N51" s="72"/>
     </row>
     <row r="52" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N52" s="73"/>
+      <c r="N52" s="72"/>
     </row>
     <row r="53" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N53" s="73"/>
+      <c r="N53" s="72"/>
     </row>
     <row r="54" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N54" s="73"/>
+      <c r="N54" s="72"/>
     </row>
     <row r="55" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N55" s="73"/>
+      <c r="N55" s="72"/>
     </row>
     <row r="56" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N56" s="73"/>
+      <c r="N56" s="72"/>
     </row>
     <row r="57" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N57" s="73"/>
+      <c r="N57" s="72"/>
     </row>
     <row r="58" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N58" s="73"/>
+      <c r="N58" s="72"/>
     </row>
     <row r="59" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N59" s="73"/>
+      <c r="N59" s="72"/>
     </row>
     <row r="60" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N60" s="73"/>
+      <c r="N60" s="72"/>
     </row>
     <row r="61" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N61" s="73"/>
+      <c r="N61" s="72"/>
     </row>
     <row r="62" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N62" s="73"/>
+      <c r="N62" s="72"/>
     </row>
     <row r="63" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N63" s="73"/>
+      <c r="N63" s="72"/>
     </row>
     <row r="64" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N64" s="73"/>
+      <c r="N64" s="72"/>
     </row>
     <row r="65" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N65" s="73"/>
+      <c r="N65" s="72"/>
     </row>
     <row r="66" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N66" s="73"/>
+      <c r="N66" s="72"/>
     </row>
     <row r="67" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N67" s="73"/>
+      <c r="N67" s="72"/>
     </row>
     <row r="68" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N68" s="73"/>
+      <c r="N68" s="72"/>
     </row>
     <row r="69" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N69" s="73"/>
+      <c r="N69" s="72"/>
     </row>
     <row r="70" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N70" s="73"/>
+      <c r="N70" s="72"/>
     </row>
     <row r="71" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N71" s="73"/>
+      <c r="N71" s="72"/>
     </row>
     <row r="72" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N72" s="73"/>
+      <c r="N72" s="72"/>
     </row>
     <row r="73" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N73" s="73"/>
+      <c r="N73" s="72"/>
     </row>
     <row r="74" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N74" s="73"/>
+      <c r="N74" s="72"/>
     </row>
     <row r="75" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N75" s="73"/>
+      <c r="N75" s="72"/>
     </row>
     <row r="76" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N76" s="73"/>
+      <c r="N76" s="72"/>
     </row>
     <row r="77" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N77" s="73"/>
+      <c r="N77" s="72"/>
     </row>
     <row r="78" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N78" s="73"/>
+      <c r="N78" s="72"/>
     </row>
     <row r="79" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N79" s="73"/>
+      <c r="N79" s="72"/>
     </row>
     <row r="80" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N80" s="73"/>
+      <c r="N80" s="72"/>
     </row>
     <row r="81" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N81" s="73"/>
+      <c r="N81" s="72"/>
     </row>
     <row r="82" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N82" s="73"/>
+      <c r="N82" s="72"/>
     </row>
     <row r="83" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N83" s="73"/>
+      <c r="N83" s="72"/>
     </row>
     <row r="84" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N84" s="73"/>
+      <c r="N84" s="72"/>
     </row>
     <row r="85" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N85" s="73"/>
+      <c r="N85" s="72"/>
     </row>
     <row r="86" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N86" s="73"/>
+      <c r="N86" s="72"/>
     </row>
     <row r="87" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N87" s="73"/>
+      <c r="N87" s="72"/>
     </row>
     <row r="88" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N88" s="73"/>
+      <c r="N88" s="72"/>
     </row>
     <row r="89" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N89" s="73"/>
+      <c r="N89" s="72"/>
     </row>
     <row r="90" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N90" s="73"/>
+      <c r="N90" s="72"/>
     </row>
     <row r="91" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N91" s="73"/>
+      <c r="N91" s="72"/>
     </row>
     <row r="92" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N92" s="73"/>
+      <c r="N92" s="72"/>
     </row>
     <row r="93" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N93" s="73"/>
+      <c r="N93" s="72"/>
     </row>
     <row r="94" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N94" s="73"/>
+      <c r="N94" s="72"/>
     </row>
     <row r="95" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N95" s="73"/>
+      <c r="N95" s="72"/>
     </row>
     <row r="96" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N96" s="73"/>
+      <c r="N96" s="72"/>
     </row>
     <row r="97" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N97" s="73"/>
+      <c r="N97" s="72"/>
     </row>
     <row r="98" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N98" s="73"/>
+      <c r="N98" s="72"/>
     </row>
     <row r="99" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N99" s="73"/>
+      <c r="N99" s="72"/>
     </row>
     <row r="100" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N100" s="73"/>
+      <c r="N100" s="72"/>
     </row>
     <row r="101" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N101" s="73"/>
+      <c r="N101" s="72"/>
     </row>
     <row r="102" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N102" s="73"/>
+      <c r="N102" s="72"/>
     </row>
     <row r="103" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N103" s="73"/>
+      <c r="N103" s="72"/>
     </row>
     <row r="104" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N104" s="73"/>
+      <c r="N104" s="72"/>
     </row>
     <row r="105" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N105" s="73"/>
+      <c r="N105" s="72"/>
     </row>
     <row r="106" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N106" s="73"/>
+      <c r="N106" s="72"/>
     </row>
     <row r="107" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N107" s="73"/>
+      <c r="N107" s="72"/>
     </row>
     <row r="108" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N108" s="73"/>
+      <c r="N108" s="72"/>
     </row>
     <row r="109" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N109" s="73"/>
+      <c r="N109" s="72"/>
     </row>
     <row r="110" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N110" s="73"/>
+      <c r="N110" s="72"/>
     </row>
     <row r="111" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N111" s="73"/>
+      <c r="N111" s="72"/>
     </row>
     <row r="112" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N112" s="73"/>
+      <c r="N112" s="72"/>
     </row>
     <row r="113" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N113" s="73"/>
+      <c r="N113" s="72"/>
     </row>
     <row r="114" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N114" s="73"/>
+      <c r="N114" s="72"/>
     </row>
     <row r="115" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N115" s="73"/>
+      <c r="N115" s="72"/>
     </row>
     <row r="116" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N116" s="73"/>
+      <c r="N116" s="72"/>
     </row>
     <row r="117" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N117" s="73"/>
+      <c r="N117" s="72"/>
     </row>
     <row r="118" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N118" s="73"/>
+      <c r="N118" s="72"/>
     </row>
     <row r="119" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N119" s="73"/>
+      <c r="N119" s="72"/>
     </row>
     <row r="120" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N120" s="73"/>
+      <c r="N120" s="72"/>
     </row>
     <row r="121" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N121" s="73"/>
+      <c r="N121" s="72"/>
     </row>
     <row r="122" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N122" s="73"/>
+      <c r="N122" s="72"/>
     </row>
     <row r="123" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N123" s="73"/>
+      <c r="N123" s="72"/>
     </row>
     <row r="124" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N124" s="73"/>
+      <c r="N124" s="72"/>
     </row>
     <row r="125" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N125" s="73"/>
+      <c r="N125" s="72"/>
     </row>
     <row r="126" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N126" s="73"/>
+      <c r="N126" s="72"/>
     </row>
     <row r="127" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N127" s="73"/>
+      <c r="N127" s="72"/>
     </row>
     <row r="128" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N128" s="73"/>
+      <c r="N128" s="72"/>
     </row>
     <row r="129" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N129" s="73"/>
+      <c r="N129" s="72"/>
     </row>
     <row r="130" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N130" s="73"/>
+      <c r="N130" s="72"/>
     </row>
     <row r="131" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N131" s="73"/>
+      <c r="N131" s="72"/>
     </row>
   </sheetData>
   <autoFilter ref="B6:D6" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <mergeCells count="2">
+    <mergeCell ref="A7:A13"/>
+    <mergeCell ref="A14:A20"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="B7:B33 B6:C6 C1:E1 C34:E65534">
-    <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="C7:D33">
+    <cfRule type="cellIs" dxfId="10" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:E1 B6:C6 C34:E65534 B7:B33">
+    <cfRule type="cellIs" dxfId="7" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:D33">
-    <cfRule type="cellIs" dxfId="7" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Low"</formula>
+  <conditionalFormatting sqref="E7:E33">
+    <cfRule type="cellIs" dxfId="4" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Red"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E7:E33">
-    <cfRule type="cellIs" dxfId="4" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Yellow"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Red"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Green"</formula>
@@ -4331,16 +4409,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L8:L33 C7:D33" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L8:L14 L15:L33 C7:D14 C15:D33" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H33" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H14 H15:H33" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>Risk_Area</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B33" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B14 B15:B33" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K33" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K14 K15:K33" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"Acceptance,Avoidance,Contingency,Mitigation,Transfer"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4367,102 +4445,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="55" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="56" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="56" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="56" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="56" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="56" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="56" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="56" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="56" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="56" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="56" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="56" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="56" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="56" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="56" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A16" s="57" t="s">
+      <c r="A16" s="56" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="56" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A18" s="57" t="s">
+      <c r="A18" s="56" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="56" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="56" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added risk status description column
</commit_message>
<xml_diff>
--- a/LCOM Documents/Iteration2/LCOMRiskList.xlsx
+++ b/LCOM Documents/Iteration2/LCOMRiskList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deepakchand/Desktop/ITC303-9-Team1-Project/LCOM Documents/Iteration2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060040F4-12CC-5B41-9510-CC0062ED0C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8D6284-A96F-664F-8B98-216D35F2906D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Risk_Tracking_Log!$B$6:$D$6</definedName>
     <definedName name="as">[1]DropDown_Elements!$A$2:$A$30</definedName>
     <definedName name="OLE_LINK1" localSheetId="1">Risk_Tracking_Log!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Risk_Tracking_Log!$A$1:$M$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Risk_Tracking_Log!$A$1:$N$24</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Risk_Tracking_Log!$1:$6</definedName>
     <definedName name="Risk_Area">DropDown_Elements!$A$2:$A$30</definedName>
   </definedNames>
@@ -441,7 +441,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
+    <comment ref="H6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -464,7 +464,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
+    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
@@ -487,7 +487,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
+    <comment ref="J6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
         <r>
           <rPr>
@@ -510,7 +510,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
+    <comment ref="K6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -533,7 +533,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
+    <comment ref="L6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -556,7 +556,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000C000000}">
+    <comment ref="M6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -579,7 +579,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
+    <comment ref="N6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -607,7 +607,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="187">
   <si>
     <t>ID</t>
   </si>
@@ -1478,6 +1478,51 @@
   </si>
   <si>
     <t>APP Specific Risks</t>
+  </si>
+  <si>
+    <t>Current status description</t>
+  </si>
+  <si>
+    <t>Due to unforseen circumstances this risk has a fair chance of occurance.</t>
+  </si>
+  <si>
+    <t>Iteration 1.1 has been completed.</t>
+  </si>
+  <si>
+    <t>Group members are using deffierent computer/laptopns, hence compatibility issues remains an open risk especially when working in version control</t>
+  </si>
+  <si>
+    <t>Scope creep continues to be a risk unless a finalised version agreed upon by the group is established.</t>
+  </si>
+  <si>
+    <t>Inconsisten communication pattern remains an open risk.</t>
+  </si>
+  <si>
+    <t>This is a generic risk associated when different operating systems are used.</t>
+  </si>
+  <si>
+    <t>The group has decided to use local storage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group members have demonstrated basic competency. However, depending on use case implementations complications can arise. </t>
+  </si>
+  <si>
+    <t>Usability will need to be implemented and tested to gain better understanding. Therefore it remains an open risk.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The app needs to be tested to see how it processes user input and generates outputs. </t>
+  </si>
+  <si>
+    <t>Current legal obligations will need to be referred to depending on how much of perfornal user data is collected/stored.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While allowing customisation such as font colour and size will be pleasing, it can cause unpredicted complications. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If time. resource, and knowledge is available, such customisation can be considere. </t>
+  </si>
+  <si>
+    <t>As each use case will get implemented, group members might have different level of skills and  knowledge of the coding language which can cause complications. Therefore this remains as an open risk.</t>
   </si>
 </sst>
 </file>
@@ -1487,7 +1532,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1602,6 +1647,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1629,7 +1679,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1690,7 +1740,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -1699,37 +1749,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1926,7 +1946,89 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -1943,140 +2045,6 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -2141,7 +2109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2173,233 +2141,212 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2505,9 +2452,9 @@
       <sheetName val="DropDown_Elements"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1">
         <row r="2">
           <cell r="A2" t="str">
             <v>Schedule</v>
@@ -2880,173 +2827,173 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" style="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="93" style="9" customWidth="1"/>
     <col min="3" max="16384" width="9.1640625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="81" t="str">
+      <c r="A1" s="72" t="str">
         <f>Risk_Tracking_Log!A1</f>
         <v>RISK MANAGEMENT LOG</v>
       </c>
-      <c r="B1" s="82"/>
+      <c r="B1" s="73"/>
     </row>
     <row r="2" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12" x14ac:dyDescent="0.15">
-      <c r="A3" s="20"/>
-      <c r="B3" s="14" t="s">
+      <c r="A3" s="18"/>
+      <c r="B3" s="12" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12" x14ac:dyDescent="0.15">
-      <c r="A4" s="18"/>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="16"/>
+      <c r="B4" s="13" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12" x14ac:dyDescent="0.15">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="43" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="48" x14ac:dyDescent="0.15">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="43" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="72" x14ac:dyDescent="0.15">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="43" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="12" x14ac:dyDescent="0.15">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="44" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.15">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="43" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="12" x14ac:dyDescent="0.15">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="43" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="12" x14ac:dyDescent="0.15">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="43" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="12" x14ac:dyDescent="0.15">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="43" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="12" x14ac:dyDescent="0.15">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="43" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12" x14ac:dyDescent="0.15">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="43" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="12" x14ac:dyDescent="0.15">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="43" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="12" x14ac:dyDescent="0.15">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="43" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="64" t="s">
+      <c r="A17" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="65" t="s">
+      <c r="B17" s="59" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="37" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="19" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="15" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="61" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="19" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3064,11 +3011,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O131"/>
+  <dimension ref="A1:P122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3078,1287 +3025,1170 @@
     <col min="3" max="3" width="10.5" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="34" style="46" customWidth="1"/>
-    <col min="8" max="8" width="22.1640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="30.83203125" style="46" customWidth="1"/>
-    <col min="11" max="11" width="12.83203125" style="46" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="30.83203125" style="46" customWidth="1"/>
-    <col min="15" max="15" width="6" customWidth="1"/>
+    <col min="6" max="8" width="34" style="42" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" style="42" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="30.83203125" style="42" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" style="42" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="30.83203125" style="42" customWidth="1"/>
+    <col min="16" max="16" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="6" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="2" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-    </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+    </row>
+    <row r="2" spans="1:16" s="1" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="7" t="str">
+      <c r="E2" s="29"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="7" t="str">
         <f>A2</f>
         <v>Project Name:</v>
       </c>
-      <c r="J2" s="29" t="str">
+      <c r="K2" s="27" t="str">
         <f>D2</f>
         <v>ADHD Task Manager</v>
       </c>
-      <c r="K2" s="35"/>
-    </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="L2" s="33"/>
+    </row>
+    <row r="3" spans="1:16" s="1" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="33" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="E3" s="35"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="8" t="str">
+      <c r="E3" s="33"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="8" t="str">
         <f>A3</f>
         <v>National Center:</v>
       </c>
-      <c r="J3" s="33" t="str">
+      <c r="K3" s="31" t="str">
         <f>D3</f>
         <v>Australia</v>
       </c>
-      <c r="K3" s="35"/>
-    </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="L3" s="33"/>
+    </row>
+    <row r="4" spans="1:16" s="1" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="36" t="s">
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="8" t="str">
+      <c r="E4" s="33"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="8" t="str">
         <f>A4</f>
         <v>Project Manager Name:</v>
       </c>
-      <c r="J4" s="36" t="str">
+      <c r="K4" s="34" t="str">
         <f>D4</f>
         <v>Team 1</v>
       </c>
-      <c r="K4" s="35"/>
-    </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" ht="61" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="L4" s="33"/>
+    </row>
+    <row r="5" spans="1:16" s="1" customFormat="1" ht="61" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="74" t="s">
+      <c r="B5" s="26"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="65" t="s">
         <v>145</v>
       </c>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="8" t="str">
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="8" t="str">
         <f>A5</f>
         <v>Project Description:</v>
       </c>
-      <c r="J5" s="49" t="str">
+      <c r="K5" s="45" t="str">
         <f>D5</f>
         <v>Task Manager app for individuals with ADHD to complete tasks, gain rewards, and stay motivated.</v>
       </c>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="51"/>
-    </row>
-    <row r="6" spans="1:15" s="3" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="53" t="s">
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="47"/>
+    </row>
+    <row r="6" spans="1:16" s="3" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="52" t="s">
+      <c r="E6" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="54" t="s">
+      <c r="F6" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="54" t="s">
+      <c r="G6" s="80" t="s">
+        <v>172</v>
+      </c>
+      <c r="H6" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="57" t="s">
+      <c r="I6" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="52" t="s">
+      <c r="J6" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="52" t="s">
+      <c r="K6" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="K6" s="52" t="s">
+      <c r="L6" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="54" t="s">
+      <c r="M6" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="M6" s="63" t="s">
+      <c r="N6" s="57" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="111" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="83" t="s">
+    <row r="7" spans="1:16" ht="111" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="74" t="s">
         <v>170</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="62" t="str">
+      <c r="E7" s="56" t="str">
         <f>IF(OR(AND(B7&lt;&gt;"Closed",C7="High",D7="High"),AND(B7&lt;&gt;"Closed",C7="High",D7="Medium"),AND(B7&lt;&gt;"Closed",C7="Medium",D7="High")),"Red",IF(OR(AND(B7&lt;&gt;"Closed",C7="High",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Medium",D7="Medium"),AND(B7&lt;&gt;"Closed",C7="Low",D7="High")),"Yellow",IF(OR(AND(B7&lt;&gt;"Closed",C7="Medium",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Low",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Low",D7="Medium")),"Green",IF(B7="Closed","Closed",""))))</f>
         <v>Yellow</v>
       </c>
-      <c r="F7" s="39" t="s">
+      <c r="F7" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="G7" s="39" t="s">
+      <c r="G7" s="81" t="s">
+        <v>186</v>
+      </c>
+      <c r="H7" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="H7" s="38" t="s">
+      <c r="I7" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="I7" s="39" t="s">
+      <c r="J7" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="J7" s="39" t="s">
+      <c r="K7" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="K7" s="70" t="s">
+      <c r="L7" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="L7" s="39" t="s">
+      <c r="M7" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="M7" s="61" t="s">
+      <c r="N7" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="O7" t="str">
+      <c r="P7" t="str">
         <f>IF(OR(AND(B7&lt;&gt;"Closed",C7="High",E7="High"), AND(B7&lt;&gt;"Closed",C7="High", E7="Medium"),AND(B7&lt;&gt;"Closed",C7="Medium",E7="High")),"Red",IF(OR(AND(B7&lt;&gt;"Closed",C7="High",E7="Low"), AND(B7&lt;&gt;"Closed",C7="Medium", E7="Medium"),AND(B7&lt;&gt;"Closed",C7="Low",E7="High")),"Yellow",IF(OR(AND(B7&lt;&gt;"Closed",C7="Medium",E7="Low"), AND(B7&lt;&gt;"Closed",C7="Low", E7="Low"),AND(B7&lt;&gt;"Closed",C7="Low",E7="Medium")),"Green","")))</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="53" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="84"/>
-      <c r="B8" s="12" t="s">
+    <row r="8" spans="1:16" ht="53" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="75"/>
+      <c r="B8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="62" t="str">
-        <f t="shared" ref="E8:E33" si="0">IF(OR(AND(B8&lt;&gt;"Closed",C8="High",D8="High"),AND(B8&lt;&gt;"Closed",C8="High",D8="Medium"),AND(B8&lt;&gt;"Closed",C8="Medium",D8="High")),"Red",IF(OR(AND(B8&lt;&gt;"Closed",C8="High",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Medium",D8="Medium"),AND(B8&lt;&gt;"Closed",C8="Low",D8="High")),"Yellow",IF(OR(AND(B8&lt;&gt;"Closed",C8="Medium",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Low",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Low",D8="Medium")),"Green",IF(B8="Closed","Closed",""))))</f>
+      <c r="E8" s="56" t="str">
+        <f t="shared" ref="E8:E24" si="0">IF(OR(AND(B8&lt;&gt;"Closed",C8="High",D8="High"),AND(B8&lt;&gt;"Closed",C8="High",D8="Medium"),AND(B8&lt;&gt;"Closed",C8="Medium",D8="High")),"Red",IF(OR(AND(B8&lt;&gt;"Closed",C8="High",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Medium",D8="Medium"),AND(B8&lt;&gt;"Closed",C8="Low",D8="High")),"Yellow",IF(OR(AND(B8&lt;&gt;"Closed",C8="Medium",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Low",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Low",D8="Medium")),"Green",IF(B8="Closed","Closed",""))))</f>
         <v>Yellow</v>
       </c>
-      <c r="F8" s="41" t="s">
+      <c r="F8" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="38" t="s">
+      <c r="G8" s="67" t="s">
+        <v>173</v>
+      </c>
+      <c r="H8" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="H8" s="38" t="s">
+      <c r="I8" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="I8" s="40" t="s">
+      <c r="J8" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="J8" s="38" t="s">
+      <c r="K8" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="K8" s="70" t="s">
+      <c r="L8" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="L8" s="67" t="s">
+      <c r="M8" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="M8" s="43" t="s">
+      <c r="N8" s="41" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="A9" s="84"/>
-      <c r="B9" s="12" t="s">
+    <row r="9" spans="1:16" ht="24" x14ac:dyDescent="0.15">
+      <c r="A9" s="75"/>
+      <c r="B9" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="60" t="s">
+      <c r="D9" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="62" t="str">
+      <c r="E9" s="56" t="str">
         <f t="shared" si="0"/>
         <v>Closed</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="G9" s="38" t="s">
+      <c r="G9" s="67" t="s">
+        <v>174</v>
+      </c>
+      <c r="H9" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="H9" s="38" t="s">
+      <c r="I9" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="I9" s="40" t="s">
+      <c r="J9" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="J9" s="38" t="s">
+      <c r="K9" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="K9" s="70" t="s">
+      <c r="L9" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="L9" s="68" t="s">
+      <c r="M9" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="M9" s="42" t="s">
+      <c r="N9" s="40" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="48" x14ac:dyDescent="0.15">
-      <c r="A10" s="84"/>
-      <c r="B10" s="12" t="s">
+    <row r="10" spans="1:16" ht="48" x14ac:dyDescent="0.15">
+      <c r="A10" s="75"/>
+      <c r="B10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="62" t="str">
+      <c r="E10" s="56" t="str">
         <f>IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="High"),AND(B10&lt;&gt;"Closed",C10="High",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="High")),"Red",IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Low",D10="High")),"Yellow",IF(OR(AND(B10&lt;&gt;"Closed",C10="Medium",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Medium")),"Green",IF(B10="Closed","Closed",""))))</f>
         <v>Red</v>
       </c>
-      <c r="F10" s="41" t="s">
+      <c r="F10" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="G10" s="38" t="s">
+      <c r="G10" s="67" t="s">
+        <v>175</v>
+      </c>
+      <c r="H10" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="H10" s="38" t="s">
+      <c r="I10" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="I10" s="40" t="s">
+      <c r="J10" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="J10" s="38" t="s">
+      <c r="K10" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="K10" s="70" t="s">
+      <c r="L10" s="62" t="s">
         <v>113</v>
       </c>
-      <c r="L10" s="67" t="s">
+      <c r="M10" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="43" t="s">
+      <c r="N10" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="N10" s="72"/>
-    </row>
-    <row r="11" spans="1:15" ht="60" x14ac:dyDescent="0.15">
-      <c r="A11" s="84"/>
-      <c r="B11" s="12" t="s">
+      <c r="O10" s="64"/>
+    </row>
+    <row r="11" spans="1:16" ht="60" x14ac:dyDescent="0.15">
+      <c r="A11" s="75"/>
+      <c r="B11" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="62" t="str">
+      <c r="E11" s="56" t="str">
         <f>IF(OR(AND(B11&lt;&gt;"Closed",C11="High",D11="High"),AND(B11&lt;&gt;"Closed",C11="High",D11="Medium"),AND(B11&lt;&gt;"Closed",C11="Medium",D11="High")),"Red",IF(OR(AND(B11&lt;&gt;"Closed",C11="High",D11="Low"),AND(B11&lt;&gt;"Closed",C11="Medium",D11="Medium"),AND(B11&lt;&gt;"Closed",C11="Low",D11="High")),"Yellow",IF(OR(AND(B11&lt;&gt;"Closed",C11="Medium",D11="Low"),AND(B11&lt;&gt;"Closed",C11="Low",D11="Low"),AND(B11&lt;&gt;"Closed",C11="Low",D11="Medium")),"Green",IF(B11="Closed","Closed",""))))</f>
         <v>Red</v>
       </c>
-      <c r="F11" s="41" t="s">
+      <c r="F11" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="G11" s="38" t="s">
+      <c r="G11" s="67" t="s">
+        <v>176</v>
+      </c>
+      <c r="H11" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="H11" s="76" t="s">
+      <c r="I11" s="67" t="s">
         <v>141</v>
       </c>
-      <c r="I11" s="40" t="s">
+      <c r="J11" s="38" t="s">
         <v>142</v>
       </c>
-      <c r="J11" s="38" t="s">
+      <c r="K11" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="K11" s="70" t="s">
+      <c r="L11" s="62" t="s">
         <v>113</v>
       </c>
-      <c r="L11" s="67" t="s">
+      <c r="M11" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="M11" s="43" t="s">
+      <c r="N11" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="N11" s="72"/>
-    </row>
-    <row r="12" spans="1:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="A12" s="84"/>
-      <c r="B12" s="12" t="s">
+      <c r="O11" s="64"/>
+    </row>
+    <row r="12" spans="1:16" ht="24" x14ac:dyDescent="0.15">
+      <c r="A12" s="75"/>
+      <c r="B12" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="62" t="str">
+      <c r="E12" s="56" t="str">
         <f>IF(OR(AND(B12&lt;&gt;"Closed",C12="High",D12="High"),AND(B12&lt;&gt;"Closed",C12="High",D12="Medium"),AND(B12&lt;&gt;"Closed",C12="Medium",D12="High")),"Red",IF(OR(AND(B12&lt;&gt;"Closed",C12="High",D12="Low"),AND(B12&lt;&gt;"Closed",C12="Medium",D12="Medium"),AND(B12&lt;&gt;"Closed",C12="Low",D12="High")),"Yellow",IF(OR(AND(B12&lt;&gt;"Closed",C12="Medium",D12="Low"),AND(B12&lt;&gt;"Closed",C12="Low",D12="Low"),AND(B12&lt;&gt;"Closed",C12="Low",D12="Medium")),"Green",IF(B12="Closed","Closed",""))))</f>
         <v>Red</v>
       </c>
-      <c r="F12" s="41" t="s">
+      <c r="F12" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="67" t="s">
+        <v>177</v>
+      </c>
+      <c r="H12" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="H12" s="38" t="s">
+      <c r="I12" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="I12" s="77" t="s">
+      <c r="J12" s="68" t="s">
         <v>164</v>
       </c>
-      <c r="J12" s="38" t="s">
+      <c r="K12" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="K12" s="70" t="s">
+      <c r="L12" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="L12" s="67" t="s">
+      <c r="M12" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="M12" s="43" t="s">
+      <c r="N12" s="41" t="s">
         <v>132</v>
       </c>
-      <c r="N12" s="72"/>
-    </row>
-    <row r="13" spans="1:15" ht="36" x14ac:dyDescent="0.15">
-      <c r="A13" s="85"/>
-      <c r="B13" s="12" t="s">
+      <c r="O12" s="64"/>
+    </row>
+    <row r="13" spans="1:16" ht="36" x14ac:dyDescent="0.15">
+      <c r="A13" s="76"/>
+      <c r="B13" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="62" t="str">
+      <c r="E13" s="56" t="str">
         <f>IF(OR(AND(B13&lt;&gt;"Closed",C13="High",D13="High"),AND(B13&lt;&gt;"Closed",C13="High",D13="Medium"),AND(B13&lt;&gt;"Closed",C13="Medium",D13="High")),"Red",IF(OR(AND(B13&lt;&gt;"Closed",C13="High",D13="Low"),AND(B13&lt;&gt;"Closed",C13="Medium",D13="Medium"),AND(B13&lt;&gt;"Closed",C13="Low",D13="High")),"Yellow",IF(OR(AND(B13&lt;&gt;"Closed",C13="Medium",D13="Low"),AND(B13&lt;&gt;"Closed",C13="Low",D13="Low"),AND(B13&lt;&gt;"Closed",C13="Low",D13="Medium")),"Green",IF(B13="Closed","Closed",""))))</f>
         <v>Red</v>
       </c>
-      <c r="F13" s="75" t="s">
+      <c r="F13" s="66" t="s">
         <v>158</v>
       </c>
-      <c r="G13" s="76" t="s">
+      <c r="G13" s="67" t="s">
+        <v>178</v>
+      </c>
+      <c r="H13" s="67" t="s">
         <v>159</v>
       </c>
-      <c r="H13" s="76" t="s">
+      <c r="I13" s="67" t="s">
         <v>160</v>
       </c>
-      <c r="I13" s="77" t="s">
+      <c r="J13" s="68" t="s">
         <v>161</v>
       </c>
-      <c r="J13" s="76" t="s">
+      <c r="K13" s="67" t="s">
         <v>162</v>
       </c>
-      <c r="K13" s="79" t="s">
+      <c r="L13" s="70" t="s">
         <v>113</v>
       </c>
-      <c r="L13" s="80" t="s">
+      <c r="M13" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="M13" s="78" t="s">
+      <c r="N13" s="69" t="s">
         <v>163</v>
       </c>
-      <c r="N13" s="72"/>
-    </row>
-    <row r="14" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="86" t="s">
+      <c r="O13" s="64"/>
+    </row>
+    <row r="14" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="77" t="s">
         <v>171</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="56" t="str">
+        <f t="shared" si="0"/>
+        <v>Closed</v>
+      </c>
+      <c r="F14" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="G14" s="67" t="s">
+        <v>179</v>
+      </c>
+      <c r="H14" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="I14" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="J14" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="K14" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="L14" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="M14" s="60" t="s">
+        <v>2</v>
+      </c>
+      <c r="N14" s="69" t="s">
+        <v>151</v>
+      </c>
+      <c r="O14" s="64"/>
+    </row>
+    <row r="15" spans="1:16" ht="36" x14ac:dyDescent="0.15">
+      <c r="A15" s="78"/>
+      <c r="B15" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C15" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="62" t="str">
-        <f t="shared" si="0"/>
-        <v>Red</v>
-      </c>
-      <c r="F14" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="G14" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="H14" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="I14" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="J14" s="38" t="s">
-        <v>104</v>
-      </c>
-      <c r="K14" s="70" t="s">
-        <v>150</v>
-      </c>
-      <c r="L14" s="67" t="s">
-        <v>2</v>
-      </c>
-      <c r="M14" s="78" t="s">
-        <v>151</v>
-      </c>
-      <c r="N14" s="72"/>
-    </row>
-    <row r="15" spans="1:15" ht="36" x14ac:dyDescent="0.15">
-      <c r="A15" s="87"/>
-      <c r="B15" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="62" t="str">
+      <c r="E15" s="56" t="str">
         <f t="shared" si="0"/>
         <v>Yellow</v>
       </c>
-      <c r="F15" s="41" t="s">
+      <c r="F15" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="G15" s="38" t="s">
+      <c r="G15" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="H15" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="H15" s="38" t="s">
+      <c r="I15" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="I15" s="40" t="s">
+      <c r="J15" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="J15" s="38" t="s">
+      <c r="K15" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="K15" s="70" t="s">
+      <c r="L15" s="62" t="s">
         <v>113</v>
       </c>
-      <c r="L15" s="67" t="s">
+      <c r="M15" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="M15" s="43" t="s">
+      <c r="N15" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="N15" s="72"/>
-    </row>
-    <row r="16" spans="1:15" ht="60" x14ac:dyDescent="0.15">
-      <c r="A16" s="87"/>
-      <c r="B16" s="12" t="s">
+      <c r="O15" s="64"/>
+    </row>
+    <row r="16" spans="1:16" ht="60" x14ac:dyDescent="0.15">
+      <c r="A16" s="78"/>
+      <c r="B16" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E16" s="62" t="str">
+      <c r="E16" s="56" t="str">
         <f>IF(OR(AND(B16&lt;&gt;"Closed",C16="High",D16="High"),AND(B16&lt;&gt;"Closed",C16="High",D16="Medium"),AND(B16&lt;&gt;"Closed",C16="Medium",D16="High")),"Red",IF(OR(AND(B16&lt;&gt;"Closed",C16="High",D16="Low"),AND(B16&lt;&gt;"Closed",C16="Medium",D16="Medium"),AND(B16&lt;&gt;"Closed",C16="Low",D16="High")),"Yellow",IF(OR(AND(B16&lt;&gt;"Closed",C16="Medium",D16="Low"),AND(B16&lt;&gt;"Closed",C16="Low",D16="Low"),AND(B16&lt;&gt;"Closed",C16="Low",D16="Medium")),"Green",IF(B16="Closed","Closed",""))))</f>
         <v>Red</v>
       </c>
-      <c r="F16" s="75" t="s">
+      <c r="F16" s="66" t="s">
         <v>152</v>
       </c>
-      <c r="G16" s="76" t="s">
+      <c r="G16" s="67" t="s">
+        <v>181</v>
+      </c>
+      <c r="H16" s="67" t="s">
         <v>153</v>
       </c>
-      <c r="H16" s="76" t="s">
+      <c r="I16" s="67" t="s">
         <v>141</v>
       </c>
-      <c r="I16" s="77" t="s">
+      <c r="J16" s="68" t="s">
         <v>155</v>
       </c>
-      <c r="J16" s="76" t="s">
+      <c r="K16" s="67" t="s">
         <v>156</v>
       </c>
-      <c r="K16" s="79" t="s">
+      <c r="L16" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="L16" s="67" t="s">
+      <c r="M16" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="M16" s="78" t="s">
+      <c r="N16" s="69" t="s">
         <v>157</v>
       </c>
-      <c r="N16" s="72"/>
-    </row>
-    <row r="17" spans="1:14" ht="36" x14ac:dyDescent="0.15">
-      <c r="A17" s="87"/>
-      <c r="B17" s="12" t="s">
+      <c r="O16" s="64"/>
+    </row>
+    <row r="17" spans="1:15" ht="24" x14ac:dyDescent="0.15">
+      <c r="A17" s="78"/>
+      <c r="B17" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="56" t="str">
+        <f>IF(OR(AND(B17&lt;&gt;"Closed",C17="High",D17="High"),AND(B17&lt;&gt;"Closed",C17="High",D17="Medium"),AND(B17&lt;&gt;"Closed",C17="Medium",D17="High")),"Red",IF(OR(AND(B17&lt;&gt;"Closed",C17="High",D17="Low"),AND(B17&lt;&gt;"Closed",C17="Medium",D17="Medium"),AND(B17&lt;&gt;"Closed",C17="Low",D17="High")),"Yellow",IF(OR(AND(B17&lt;&gt;"Closed",C17="Medium",D17="Low"),AND(B17&lt;&gt;"Closed",C17="Low",D17="Low"),AND(B17&lt;&gt;"Closed",C17="Low",D17="Medium")),"Green",IF(B17="Closed","Closed",""))))</f>
+        <v>Red</v>
+      </c>
+      <c r="F17" s="66" t="s">
+        <v>165</v>
+      </c>
+      <c r="G17" s="67" t="s">
+        <v>182</v>
+      </c>
+      <c r="H17" s="67" t="s">
+        <v>146</v>
+      </c>
+      <c r="I17" s="67" t="s">
+        <v>154</v>
+      </c>
+      <c r="J17" s="68" t="s">
+        <v>147</v>
+      </c>
+      <c r="K17" s="67" t="s">
+        <v>148</v>
+      </c>
+      <c r="L17" s="62" t="s">
+        <v>113</v>
+      </c>
+      <c r="M17" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="N17" s="69" t="s">
+        <v>149</v>
+      </c>
+      <c r="O17" s="64"/>
+    </row>
+    <row r="18" spans="1:15" ht="36" x14ac:dyDescent="0.15">
+      <c r="A18" s="78"/>
+      <c r="B18" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="62" t="str">
+      <c r="E18" s="56" t="str">
         <f t="shared" si="0"/>
         <v>Yellow</v>
       </c>
-      <c r="F17" s="41" t="s">
+      <c r="F18" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="G17" s="38" t="s">
+      <c r="G18" s="67" t="s">
+        <v>183</v>
+      </c>
+      <c r="H18" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="H17" s="38" t="s">
+      <c r="I18" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="I17" s="40" t="s">
+      <c r="J18" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="J17" s="38" t="s">
+      <c r="K18" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="K17" s="70" t="s">
+      <c r="L18" s="62" t="s">
         <v>113</v>
       </c>
-      <c r="L17" s="67" t="s">
+      <c r="M18" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="M17" s="43" t="s">
+      <c r="N18" s="41" t="s">
         <v>138</v>
       </c>
-      <c r="N17" s="72"/>
-    </row>
-    <row r="18" spans="1:14" ht="24" x14ac:dyDescent="0.15">
-      <c r="A18" s="87"/>
-      <c r="B18" s="12" t="s">
+      <c r="O18" s="64"/>
+    </row>
+    <row r="19" spans="1:15" ht="24" x14ac:dyDescent="0.15">
+      <c r="A19" s="78"/>
+      <c r="B19" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="62" t="str">
-        <f t="shared" si="0"/>
-        <v>Red</v>
-      </c>
-      <c r="F18" s="75" t="s">
-        <v>165</v>
-      </c>
-      <c r="G18" s="76" t="s">
-        <v>146</v>
-      </c>
-      <c r="H18" s="76" t="s">
-        <v>154</v>
-      </c>
-      <c r="I18" s="77" t="s">
-        <v>147</v>
-      </c>
-      <c r="J18" s="76" t="s">
-        <v>148</v>
-      </c>
-      <c r="K18" s="70" t="s">
-        <v>113</v>
-      </c>
-      <c r="L18" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="M18" s="78" t="s">
-        <v>149</v>
-      </c>
-      <c r="N18" s="72"/>
-    </row>
-    <row r="19" spans="1:14" ht="24" x14ac:dyDescent="0.15">
-      <c r="A19" s="87"/>
-      <c r="B19" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="D19" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="62" t="str">
+      <c r="E19" s="56" t="str">
         <f>IF(OR(AND(B19&lt;&gt;"Closed",C19="High",D19="High"),AND(B19&lt;&gt;"Closed",C19="High",D19="Medium"),AND(B19&lt;&gt;"Closed",C19="Medium",D19="High")),"Red",IF(OR(AND(B19&lt;&gt;"Closed",C19="High",D19="Low"),AND(B19&lt;&gt;"Closed",C19="Medium",D19="Medium"),AND(B19&lt;&gt;"Closed",C19="Low",D19="High")),"Yellow",IF(OR(AND(B19&lt;&gt;"Closed",C19="Medium",D19="Low"),AND(B19&lt;&gt;"Closed",C19="Low",D19="Low"),AND(B19&lt;&gt;"Closed",C19="Low",D19="Medium")),"Green",IF(B19="Closed","Closed",""))))</f>
         <v>Green</v>
       </c>
-      <c r="F19" s="75" t="s">
+      <c r="F19" s="66" t="s">
         <v>166</v>
       </c>
-      <c r="G19" s="76" t="s">
+      <c r="G19" s="67" t="s">
+        <v>184</v>
+      </c>
+      <c r="H19" s="67" t="s">
         <v>167</v>
       </c>
-      <c r="H19" s="38" t="s">
+      <c r="I19" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="I19" s="77" t="s">
+      <c r="J19" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="J19" s="38" t="s">
+      <c r="K19" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="K19" s="70" t="s">
+      <c r="L19" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="L19" s="67" t="s">
+      <c r="M19" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="M19" s="78" t="s">
+      <c r="N19" s="69" t="s">
         <v>168</v>
       </c>
-      <c r="N19" s="72"/>
-    </row>
-    <row r="20" spans="1:14" ht="24" x14ac:dyDescent="0.15">
-      <c r="A20" s="88"/>
-      <c r="B20" s="12" t="s">
+      <c r="O19" s="64"/>
+    </row>
+    <row r="20" spans="1:15" ht="24" x14ac:dyDescent="0.15">
+      <c r="A20" s="79"/>
+      <c r="B20" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E20" s="62" t="str">
+      <c r="E20" s="56" t="str">
         <f>IF(OR(AND(B20&lt;&gt;"Closed",C20="High",D20="High"),AND(B20&lt;&gt;"Closed",C20="High",D20="Medium"),AND(B20&lt;&gt;"Closed",C20="Medium",D20="High")),"Red",IF(OR(AND(B20&lt;&gt;"Closed",C20="High",D20="Low"),AND(B20&lt;&gt;"Closed",C20="Medium",D20="Medium"),AND(B20&lt;&gt;"Closed",C20="Low",D20="High")),"Yellow",IF(OR(AND(B20&lt;&gt;"Closed",C20="Medium",D20="Low"),AND(B20&lt;&gt;"Closed",C20="Low",D20="Low"),AND(B20&lt;&gt;"Closed",C20="Low",D20="Medium")),"Green",IF(B20="Closed","Closed",""))))</f>
         <v>Yellow</v>
       </c>
-      <c r="F20" s="75" t="s">
+      <c r="F20" s="66" t="s">
         <v>169</v>
       </c>
-      <c r="G20" s="38" t="s">
+      <c r="G20" s="67" t="s">
+        <v>185</v>
+      </c>
+      <c r="H20" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="H20" s="38" t="s">
+      <c r="I20" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="I20" s="40" t="s">
+      <c r="J20" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="J20" s="38" t="s">
+      <c r="K20" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="K20" s="70" t="s">
+      <c r="L20" s="62" t="s">
         <v>119</v>
       </c>
-      <c r="L20" s="67" t="s">
+      <c r="M20" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="M20" s="43" t="s">
+      <c r="N20" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="N20" s="72"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O20" s="64"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A21" s="10"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="62" t="str">
+      <c r="B21" s="11"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="56" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F21" s="41"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="40"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
       <c r="J21" s="38"/>
-      <c r="K21" s="70"/>
-      <c r="L21" s="67"/>
-      <c r="M21" s="43"/>
-      <c r="N21" s="72"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="K21" s="36"/>
+      <c r="L21" s="62"/>
+      <c r="M21" s="60"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="64"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A22" s="10"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="62" t="str">
+      <c r="B22" s="11"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="56" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F22" s="41"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="40"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
       <c r="J22" s="38"/>
-      <c r="K22" s="70"/>
-      <c r="L22" s="67"/>
-      <c r="M22" s="43"/>
-      <c r="N22" s="72"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="K22" s="36"/>
+      <c r="L22" s="62"/>
+      <c r="M22" s="60"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="64"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A23" s="10"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="62" t="str">
+      <c r="B23" s="11"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="56" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F23" s="41"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="40"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
       <c r="J23" s="38"/>
-      <c r="K23" s="70"/>
-      <c r="L23" s="67"/>
-      <c r="M23" s="43"/>
-      <c r="N23" s="72"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="K23" s="36"/>
+      <c r="L23" s="62"/>
+      <c r="M23" s="60"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="64"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A24" s="10"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="62" t="str">
+      <c r="B24" s="11"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="56" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F24" s="41"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="40"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
       <c r="J24" s="38"/>
-      <c r="K24" s="70"/>
-      <c r="L24" s="67"/>
-      <c r="M24" s="43"/>
-      <c r="N24" s="72"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A25" s="10"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="62" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F25" s="41"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="70"/>
-      <c r="L25" s="67"/>
-      <c r="M25" s="43"/>
-      <c r="N25" s="72"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A26" s="10"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="62" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F26" s="41"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="40"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="70"/>
-      <c r="L26" s="67"/>
-      <c r="M26" s="43"/>
-      <c r="N26" s="72"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A27" s="10"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="62" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F27" s="41"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="40"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="70"/>
-      <c r="L27" s="67"/>
-      <c r="M27" s="43"/>
-      <c r="N27" s="72"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A28" s="10"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="62" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F28" s="41"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="40"/>
-      <c r="J28" s="38"/>
-      <c r="K28" s="70"/>
-      <c r="L28" s="67"/>
-      <c r="M28" s="43"/>
-      <c r="N28" s="72"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A29" s="10"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="62" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F29" s="41"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="38"/>
-      <c r="K29" s="70"/>
-      <c r="L29" s="67"/>
-      <c r="M29" s="43"/>
-      <c r="N29" s="72"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A30" s="10"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="62" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F30" s="41"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="70"/>
-      <c r="L30" s="67"/>
-      <c r="M30" s="43"/>
-      <c r="N30" s="72"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A31" s="10"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="62" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F31" s="41"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="38"/>
-      <c r="K31" s="70"/>
-      <c r="L31" s="67"/>
-      <c r="M31" s="43"/>
-      <c r="N31" s="72"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A32" s="10"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="62" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F32" s="41"/>
-      <c r="G32" s="38"/>
-      <c r="H32" s="38"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="38"/>
-      <c r="K32" s="70"/>
-      <c r="L32" s="67"/>
-      <c r="M32" s="43"/>
-      <c r="N32" s="72"/>
-    </row>
-    <row r="33" spans="1:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="11"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="58"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F33" s="44"/>
-      <c r="G33" s="59"/>
-      <c r="H33" s="59"/>
-      <c r="I33" s="44"/>
-      <c r="J33" s="73"/>
-      <c r="K33" s="66"/>
-      <c r="L33" s="69"/>
-      <c r="M33" s="45"/>
-      <c r="N33" s="72"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N34" s="72"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N35" s="72"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N36" s="72"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N37" s="72"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N38" s="72"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N39" s="72"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N40" s="72"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N41" s="72"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N42" s="72"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N43" s="72"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N44" s="72"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N45" s="72"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N46" s="72"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N47" s="72"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="N48" s="72"/>
-    </row>
-    <row r="49" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N49" s="72"/>
-    </row>
-    <row r="50" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N50" s="72"/>
-    </row>
-    <row r="51" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N51" s="72"/>
-    </row>
-    <row r="52" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N52" s="72"/>
-    </row>
-    <row r="53" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N53" s="72"/>
-    </row>
-    <row r="54" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N54" s="72"/>
-    </row>
-    <row r="55" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N55" s="72"/>
-    </row>
-    <row r="56" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N56" s="72"/>
-    </row>
-    <row r="57" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N57" s="72"/>
-    </row>
-    <row r="58" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N58" s="72"/>
-    </row>
-    <row r="59" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N59" s="72"/>
-    </row>
-    <row r="60" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N60" s="72"/>
-    </row>
-    <row r="61" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N61" s="72"/>
-    </row>
-    <row r="62" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N62" s="72"/>
-    </row>
-    <row r="63" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N63" s="72"/>
-    </row>
-    <row r="64" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N64" s="72"/>
-    </row>
-    <row r="65" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N65" s="72"/>
-    </row>
-    <row r="66" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N66" s="72"/>
-    </row>
-    <row r="67" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N67" s="72"/>
-    </row>
-    <row r="68" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N68" s="72"/>
-    </row>
-    <row r="69" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N69" s="72"/>
-    </row>
-    <row r="70" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N70" s="72"/>
-    </row>
-    <row r="71" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N71" s="72"/>
-    </row>
-    <row r="72" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N72" s="72"/>
-    </row>
-    <row r="73" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N73" s="72"/>
-    </row>
-    <row r="74" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N74" s="72"/>
-    </row>
-    <row r="75" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N75" s="72"/>
-    </row>
-    <row r="76" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N76" s="72"/>
-    </row>
-    <row r="77" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N77" s="72"/>
-    </row>
-    <row r="78" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N78" s="72"/>
-    </row>
-    <row r="79" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N79" s="72"/>
-    </row>
-    <row r="80" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N80" s="72"/>
-    </row>
-    <row r="81" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N81" s="72"/>
-    </row>
-    <row r="82" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N82" s="72"/>
-    </row>
-    <row r="83" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N83" s="72"/>
-    </row>
-    <row r="84" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N84" s="72"/>
-    </row>
-    <row r="85" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N85" s="72"/>
-    </row>
-    <row r="86" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N86" s="72"/>
-    </row>
-    <row r="87" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N87" s="72"/>
-    </row>
-    <row r="88" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N88" s="72"/>
-    </row>
-    <row r="89" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N89" s="72"/>
-    </row>
-    <row r="90" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N90" s="72"/>
-    </row>
-    <row r="91" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N91" s="72"/>
-    </row>
-    <row r="92" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N92" s="72"/>
-    </row>
-    <row r="93" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N93" s="72"/>
-    </row>
-    <row r="94" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N94" s="72"/>
-    </row>
-    <row r="95" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N95" s="72"/>
-    </row>
-    <row r="96" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N96" s="72"/>
-    </row>
-    <row r="97" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N97" s="72"/>
-    </row>
-    <row r="98" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N98" s="72"/>
-    </row>
-    <row r="99" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N99" s="72"/>
-    </row>
-    <row r="100" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N100" s="72"/>
-    </row>
-    <row r="101" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N101" s="72"/>
-    </row>
-    <row r="102" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N102" s="72"/>
-    </row>
-    <row r="103" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N103" s="72"/>
-    </row>
-    <row r="104" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N104" s="72"/>
-    </row>
-    <row r="105" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N105" s="72"/>
-    </row>
-    <row r="106" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N106" s="72"/>
-    </row>
-    <row r="107" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N107" s="72"/>
-    </row>
-    <row r="108" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N108" s="72"/>
-    </row>
-    <row r="109" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N109" s="72"/>
-    </row>
-    <row r="110" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N110" s="72"/>
-    </row>
-    <row r="111" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N111" s="72"/>
-    </row>
-    <row r="112" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N112" s="72"/>
-    </row>
-    <row r="113" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N113" s="72"/>
-    </row>
-    <row r="114" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N114" s="72"/>
-    </row>
-    <row r="115" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N115" s="72"/>
-    </row>
-    <row r="116" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N116" s="72"/>
-    </row>
-    <row r="117" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N117" s="72"/>
-    </row>
-    <row r="118" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N118" s="72"/>
-    </row>
-    <row r="119" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N119" s="72"/>
-    </row>
-    <row r="120" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N120" s="72"/>
-    </row>
-    <row r="121" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N121" s="72"/>
-    </row>
-    <row r="122" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N122" s="72"/>
-    </row>
-    <row r="123" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N123" s="72"/>
-    </row>
-    <row r="124" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N124" s="72"/>
-    </row>
-    <row r="125" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N125" s="72"/>
-    </row>
-    <row r="126" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N126" s="72"/>
-    </row>
-    <row r="127" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N127" s="72"/>
-    </row>
-    <row r="128" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N128" s="72"/>
-    </row>
-    <row r="129" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N129" s="72"/>
-    </row>
-    <row r="130" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N130" s="72"/>
-    </row>
-    <row r="131" spans="14:14" x14ac:dyDescent="0.15">
-      <c r="N131" s="72"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="62"/>
+      <c r="M24" s="60"/>
+      <c r="N24" s="41"/>
+      <c r="O24" s="64"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="O25" s="64"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="O26" s="64"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="O27" s="64"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="O28" s="64"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="O29" s="64"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="O30" s="64"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="O31" s="64"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="O32" s="64"/>
+    </row>
+    <row r="33" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O33" s="64"/>
+    </row>
+    <row r="34" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O34" s="64"/>
+    </row>
+    <row r="35" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O35" s="64"/>
+    </row>
+    <row r="36" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O36" s="64"/>
+    </row>
+    <row r="37" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O37" s="64"/>
+    </row>
+    <row r="38" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O38" s="64"/>
+    </row>
+    <row r="39" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O39" s="64"/>
+    </row>
+    <row r="40" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O40" s="64"/>
+    </row>
+    <row r="41" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O41" s="64"/>
+    </row>
+    <row r="42" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O42" s="64"/>
+    </row>
+    <row r="43" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O43" s="64"/>
+    </row>
+    <row r="44" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O44" s="64"/>
+    </row>
+    <row r="45" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O45" s="64"/>
+    </row>
+    <row r="46" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O46" s="64"/>
+    </row>
+    <row r="47" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O47" s="64"/>
+    </row>
+    <row r="48" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O48" s="64"/>
+    </row>
+    <row r="49" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O49" s="64"/>
+    </row>
+    <row r="50" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O50" s="64"/>
+    </row>
+    <row r="51" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O51" s="64"/>
+    </row>
+    <row r="52" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O52" s="64"/>
+    </row>
+    <row r="53" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O53" s="64"/>
+    </row>
+    <row r="54" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O54" s="64"/>
+    </row>
+    <row r="55" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O55" s="64"/>
+    </row>
+    <row r="56" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O56" s="64"/>
+    </row>
+    <row r="57" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O57" s="64"/>
+    </row>
+    <row r="58" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O58" s="64"/>
+    </row>
+    <row r="59" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O59" s="64"/>
+    </row>
+    <row r="60" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O60" s="64"/>
+    </row>
+    <row r="61" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O61" s="64"/>
+    </row>
+    <row r="62" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O62" s="64"/>
+    </row>
+    <row r="63" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O63" s="64"/>
+    </row>
+    <row r="64" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O64" s="64"/>
+    </row>
+    <row r="65" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O65" s="64"/>
+    </row>
+    <row r="66" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O66" s="64"/>
+    </row>
+    <row r="67" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O67" s="64"/>
+    </row>
+    <row r="68" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O68" s="64"/>
+    </row>
+    <row r="69" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O69" s="64"/>
+    </row>
+    <row r="70" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O70" s="64"/>
+    </row>
+    <row r="71" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O71" s="64"/>
+    </row>
+    <row r="72" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O72" s="64"/>
+    </row>
+    <row r="73" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O73" s="64"/>
+    </row>
+    <row r="74" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O74" s="64"/>
+    </row>
+    <row r="75" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O75" s="64"/>
+    </row>
+    <row r="76" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O76" s="64"/>
+    </row>
+    <row r="77" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O77" s="64"/>
+    </row>
+    <row r="78" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O78" s="64"/>
+    </row>
+    <row r="79" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O79" s="64"/>
+    </row>
+    <row r="80" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O80" s="64"/>
+    </row>
+    <row r="81" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O81" s="64"/>
+    </row>
+    <row r="82" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O82" s="64"/>
+    </row>
+    <row r="83" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O83" s="64"/>
+    </row>
+    <row r="84" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O84" s="64"/>
+    </row>
+    <row r="85" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O85" s="64"/>
+    </row>
+    <row r="86" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O86" s="64"/>
+    </row>
+    <row r="87" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O87" s="64"/>
+    </row>
+    <row r="88" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O88" s="64"/>
+    </row>
+    <row r="89" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O89" s="64"/>
+    </row>
+    <row r="90" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O90" s="64"/>
+    </row>
+    <row r="91" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O91" s="64"/>
+    </row>
+    <row r="92" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O92" s="64"/>
+    </row>
+    <row r="93" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O93" s="64"/>
+    </row>
+    <row r="94" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O94" s="64"/>
+    </row>
+    <row r="95" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O95" s="64"/>
+    </row>
+    <row r="96" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O96" s="64"/>
+    </row>
+    <row r="97" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O97" s="64"/>
+    </row>
+    <row r="98" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O98" s="64"/>
+    </row>
+    <row r="99" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O99" s="64"/>
+    </row>
+    <row r="100" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O100" s="64"/>
+    </row>
+    <row r="101" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O101" s="64"/>
+    </row>
+    <row r="102" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O102" s="64"/>
+    </row>
+    <row r="103" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O103" s="64"/>
+    </row>
+    <row r="104" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O104" s="64"/>
+    </row>
+    <row r="105" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O105" s="64"/>
+    </row>
+    <row r="106" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O106" s="64"/>
+    </row>
+    <row r="107" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O107" s="64"/>
+    </row>
+    <row r="108" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O108" s="64"/>
+    </row>
+    <row r="109" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O109" s="64"/>
+    </row>
+    <row r="110" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O110" s="64"/>
+    </row>
+    <row r="111" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O111" s="64"/>
+    </row>
+    <row r="112" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O112" s="64"/>
+    </row>
+    <row r="113" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O113" s="64"/>
+    </row>
+    <row r="114" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O114" s="64"/>
+    </row>
+    <row r="115" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O115" s="64"/>
+    </row>
+    <row r="116" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O116" s="64"/>
+    </row>
+    <row r="117" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O117" s="64"/>
+    </row>
+    <row r="118" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O118" s="64"/>
+    </row>
+    <row r="119" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O119" s="64"/>
+    </row>
+    <row r="120" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O120" s="64"/>
+    </row>
+    <row r="121" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O121" s="64"/>
+    </row>
+    <row r="122" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O122" s="64"/>
     </row>
   </sheetData>
   <autoFilter ref="B6:D6" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
@@ -4367,7 +4197,7 @@
     <mergeCell ref="A14:A20"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="C7:D33">
+  <conditionalFormatting sqref="C7:D24">
     <cfRule type="cellIs" dxfId="10" priority="9" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
@@ -4378,7 +4208,7 @@
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:E1 B6:C6 C34:E65534 B7:B33">
+  <conditionalFormatting sqref="C1:E1 B6:C6 C25:E65525 B7:B24">
     <cfRule type="cellIs" dxfId="7" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
@@ -4389,7 +4219,7 @@
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7:E33">
+  <conditionalFormatting sqref="E7:E24">
     <cfRule type="cellIs" dxfId="4" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Red"</formula>
     </cfRule>
@@ -4400,7 +4230,7 @@
       <formula>"Green"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:L33">
+  <conditionalFormatting sqref="M8:M24">
     <cfRule type="cellIs" dxfId="1" priority="4" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
@@ -4409,16 +4239,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L8:L14 L15:L33 C7:D14 C15:D33" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19:D24 C7:D18 M19:M24 M8:M18" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H14 H15:H33" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I19:I24 I7:I18" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>Risk_Area</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B14 B15:B33" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19:B24 B7:B18" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K14 K15:K33" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L19:L24 L7:L18" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"Acceptance,Avoidance,Contingency,Mitigation,Transfer"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4445,102 +4275,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="51" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="52" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="52" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="52" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="52" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="52" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="52" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="52" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="52" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="52" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="52" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A12" s="56" t="s">
+      <c r="A12" s="52" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A13" s="56" t="s">
+      <c r="A13" s="52" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A14" s="56" t="s">
+      <c r="A14" s="52" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="52" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A16" s="56" t="s">
+      <c r="A16" s="52" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="52" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A18" s="56" t="s">
+      <c r="A18" s="52" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A19" s="56" t="s">
+      <c r="A19" s="52" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="52" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>